<commit_message>
Added all record header fields from .xlsx
still need the output values and management.
</commit_message>
<xml_diff>
--- a/CombSpillageCode.xlsx
+++ b/CombSpillageCode.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
@@ -12,7 +12,7 @@
     <sheet name="DataParameters" sheetId="2" r:id="rId3"/>
     <sheet name="DiagnosticsData" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -22,7 +22,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="AK12" authorId="0">
+    <comment ref="AK12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2093" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2121" uniqueCount="474">
   <si>
     <t>Second</t>
   </si>
@@ -1110,24 +1110,12 @@
 _max</t>
   </si>
   <si>
-    <t>num_rec</t>
-  </si>
-  <si>
     <t>Incremented for each record.  Start from 1 on any code re-start.</t>
   </si>
   <si>
     <t>Place holder for extra temp</t>
   </si>
   <si>
-    <t>niu_a</t>
-  </si>
-  <si>
-    <t>niu_b</t>
-  </si>
-  <si>
-    <t>niu_c</t>
-  </si>
-  <si>
     <t>avg</t>
   </si>
   <si>
@@ -1242,15 +1230,6 @@
     <t>sec_co2</t>
   </si>
   <si>
-    <t>ppm_co2zone</t>
-  </si>
-  <si>
-    <t>ppm_co2zone_min</t>
-  </si>
-  <si>
-    <t>ppm_co2zone_max</t>
-  </si>
-  <si>
     <t>sec_p</t>
   </si>
   <si>
@@ -1263,24 +1242,6 @@
     <t>p_whvent</t>
   </si>
   <si>
-    <t>ppm_co2wh</t>
-  </si>
-  <si>
-    <t>ppm_co2wh_min</t>
-  </si>
-  <si>
-    <t>ppm_co2wh_max</t>
-  </si>
-  <si>
-    <t>ppm_co2f</t>
-  </si>
-  <si>
-    <t>ppm_co2f_min</t>
-  </si>
-  <si>
-    <t>ppm_co2f_max</t>
-  </si>
-  <si>
     <t>p_whvent_rng</t>
   </si>
   <si>
@@ -1344,9 +1305,6 @@
     <t>max</t>
   </si>
   <si>
-    <t>NAN</t>
-  </si>
-  <si>
     <t>These are placeholders for a possible added temperature</t>
   </si>
   <si>
@@ -1396,6 +1354,129 @@
   </si>
   <si>
     <t>Same as above</t>
+  </si>
+  <si>
+    <t>t_extra</t>
+  </si>
+  <si>
+    <t>t_extra_min</t>
+  </si>
+  <si>
+    <t>t_extra_max</t>
+  </si>
+  <si>
+    <t>site</t>
+  </si>
+  <si>
+    <t>rec_num</t>
+  </si>
+  <si>
+    <t>loc_co2</t>
+  </si>
+  <si>
+    <t>loc_p</t>
+  </si>
+  <si>
+    <t>ppm_co2_whvent</t>
+  </si>
+  <si>
+    <t>ppm_co2_whvent_min</t>
+  </si>
+  <si>
+    <t>ppm_co2_whvent_max</t>
+  </si>
+  <si>
+    <t>ppm_co2_fvent</t>
+  </si>
+  <si>
+    <t>ppm_co2_fvent_min</t>
+  </si>
+  <si>
+    <t>ppm_co2_fvent_max</t>
+  </si>
+  <si>
+    <t>ppm_co2_zone</t>
+  </si>
+  <si>
+    <t>ppm_co2_zone_min</t>
+  </si>
+  <si>
+    <t>ppm_co2_zone_max</t>
+  </si>
+  <si>
+    <t>p_zero_min</t>
+  </si>
+  <si>
+    <t>p_zero_max</t>
+  </si>
+  <si>
+    <t>p_zero_rng_min</t>
+  </si>
+  <si>
+    <t>p_zero_rng_max</t>
+  </si>
+  <si>
+    <t>p_whvent_min</t>
+  </si>
+  <si>
+    <t>p_whvent_max</t>
+  </si>
+  <si>
+    <t>p_whvent_rng_min</t>
+  </si>
+  <si>
+    <t>p_whvent_rng_max</t>
+  </si>
+  <si>
+    <t>p_fvent_min</t>
+  </si>
+  <si>
+    <t>p_fvent_max</t>
+  </si>
+  <si>
+    <t>p_fvent_rng_min</t>
+  </si>
+  <si>
+    <t>p_fvent_rng_max</t>
+  </si>
+  <si>
+    <t>p_zone_min</t>
+  </si>
+  <si>
+    <t>p_zone_max</t>
+  </si>
+  <si>
+    <t>p_zone_rng_min</t>
+  </si>
+  <si>
+    <t>p_zone_rng_max</t>
+  </si>
+  <si>
+    <t>wh_status</t>
+  </si>
+  <si>
+    <t>f_status</t>
+  </si>
+  <si>
+    <t>wh_mode</t>
+  </si>
+  <si>
+    <t>f_mode</t>
+  </si>
+  <si>
+    <t>sys_state</t>
+  </si>
+  <si>
+    <t>scans_accum</t>
+  </si>
+  <si>
+    <t>sec_whcooldown</t>
+  </si>
+  <si>
+    <t>sec_fcooldown</t>
+  </si>
+  <si>
+    <t>sec_count</t>
   </si>
 </sst>
 </file>
@@ -1506,7 +1587,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1567,6 +1648,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1610,7 +1703,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1804,12 +1897,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1829,6 +1916,24 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1846,6 +1951,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1894,7 +2002,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1929,7 +2037,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2310,18 +2418,18 @@
       <c r="D4" s="51"/>
       <c r="E4" s="51"/>
       <c r="F4" s="51"/>
-      <c r="G4" s="71" t="s">
+      <c r="G4" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="78"/>
+      <c r="J4" s="78"/>
       <c r="K4" s="51"/>
-      <c r="L4" s="71" t="s">
+      <c r="L4" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="71"/>
-      <c r="N4" s="71"/>
+      <c r="M4" s="78"/>
+      <c r="N4" s="78"/>
       <c r="O4" s="51"/>
       <c r="P4" s="51"/>
       <c r="R4" s="7"/>
@@ -2330,10 +2438,10 @@
       <c r="U4" s="7"/>
       <c r="V4" s="7"/>
       <c r="W4" s="7"/>
-      <c r="X4" s="72" t="s">
+      <c r="X4" s="79" t="s">
         <v>53</v>
       </c>
-      <c r="Y4" s="72"/>
+      <c r="Y4" s="79"/>
       <c r="Z4" s="7"/>
       <c r="AA4" s="7"/>
       <c r="AB4" s="7"/>
@@ -2345,10 +2453,10 @@
       <c r="AH4" s="7"/>
       <c r="AI4" s="7"/>
       <c r="AJ4" s="7"/>
-      <c r="AK4" s="72" t="s">
+      <c r="AK4" s="79" t="s">
         <v>53</v>
       </c>
-      <c r="AL4" s="72"/>
+      <c r="AL4" s="79"/>
       <c r="AM4" s="7"/>
       <c r="AN4" s="7"/>
       <c r="AO4" s="7"/>
@@ -12157,16 +12265,16 @@
   <dimension ref="A1:H328"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozenSplit"/>
+      <pane ySplit="4" topLeftCell="A119" activePane="bottomLeft" state="frozenSplit"/>
       <selection sqref="A1:A1048576"/>
-      <selection pane="bottomLeft" activeCell="I76" sqref="I76"/>
+      <selection pane="bottomLeft" activeCell="C136" sqref="C136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.7109375" style="16" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" customWidth="1"/>
     <col min="4" max="5" width="9.140625" style="17"/>
     <col min="6" max="6" width="64" style="47" customWidth="1"/>
   </cols>
@@ -12187,16 +12295,16 @@
         <v>274</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>435</v>
+        <v>421</v>
       </c>
       <c r="C4" s="56" t="s">
-        <v>424</v>
+        <v>411</v>
       </c>
       <c r="D4" s="70" t="s">
-        <v>425</v>
+        <v>412</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>431</v>
+        <v>417</v>
       </c>
       <c r="F4" s="68" t="s">
         <v>39</v>
@@ -12204,7 +12312,7 @@
     </row>
     <row r="5" spans="1:6" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="40"/>
-      <c r="B5" s="73"/>
+      <c r="B5" s="71"/>
       <c r="C5" s="44"/>
       <c r="F5" s="44"/>
     </row>
@@ -12212,13 +12320,15 @@
       <c r="A6" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="73"/>
-      <c r="C6" s="44"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="44" t="s">
+        <v>436</v>
+      </c>
       <c r="D6" s="41" t="s">
-        <v>433</v>
+        <v>419</v>
       </c>
       <c r="E6" s="41" t="s">
-        <v>433</v>
+        <v>419</v>
       </c>
       <c r="F6" s="44"/>
     </row>
@@ -12226,43 +12336,43 @@
       <c r="A7" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="73" t="s">
+      <c r="B7" s="71" t="s">
         <v>87</v>
       </c>
       <c r="C7" s="44" t="s">
         <v>87</v>
       </c>
       <c r="D7" s="41" t="s">
-        <v>433</v>
+        <v>419</v>
       </c>
       <c r="E7" s="41" t="s">
         <v>86</v>
       </c>
       <c r="F7" s="44" t="s">
-        <v>436</v>
+        <v>422</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="B8" s="73"/>
+      <c r="B8" s="71"/>
       <c r="C8" s="44" t="s">
+        <v>437</v>
+      </c>
+      <c r="D8" s="41" t="s">
+        <v>419</v>
+      </c>
+      <c r="E8" s="41" t="s">
+        <v>419</v>
+      </c>
+      <c r="F8" s="44" t="s">
         <v>351</v>
-      </c>
-      <c r="D8" s="41" t="s">
-        <v>433</v>
-      </c>
-      <c r="E8" s="41" t="s">
-        <v>433</v>
-      </c>
-      <c r="F8" s="44" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="40"/>
-      <c r="B9" s="73"/>
+      <c r="B9" s="71"/>
       <c r="C9" s="44"/>
       <c r="D9" s="41"/>
       <c r="E9" s="41"/>
@@ -12272,45 +12382,45 @@
       <c r="A10" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="B10" s="74" t="s">
+      <c r="B10" s="72" t="s">
         <v>119</v>
       </c>
       <c r="C10" s="46" t="s">
         <v>295</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F10" s="47"/>
     </row>
     <row r="11" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
-      <c r="B11" s="74"/>
+      <c r="B11" s="72"/>
       <c r="C11" s="46" t="s">
         <v>296</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="F11" s="47"/>
     </row>
     <row r="12" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
-      <c r="B12" s="74"/>
+      <c r="B12" s="72"/>
       <c r="C12" s="46" t="s">
         <v>297</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="F12" s="47"/>
     </row>
@@ -12318,45 +12428,45 @@
       <c r="A13" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="B13" s="74" t="s">
+      <c r="B13" s="72" t="s">
         <v>120</v>
       </c>
       <c r="C13" s="46" t="s">
         <v>298</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F13" s="47"/>
     </row>
     <row r="14" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
-      <c r="B14" s="74"/>
+      <c r="B14" s="72"/>
       <c r="C14" s="46" t="s">
         <v>299</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="F14" s="47"/>
     </row>
     <row r="15" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
-      <c r="B15" s="74"/>
+      <c r="B15" s="72"/>
       <c r="C15" s="46" t="s">
         <v>300</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="F15" s="47"/>
     </row>
@@ -12364,45 +12474,45 @@
       <c r="A16" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="B16" s="74" t="s">
+      <c r="B16" s="72" t="s">
         <v>121</v>
       </c>
       <c r="C16" s="46" t="s">
         <v>301</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F16" s="47"/>
     </row>
     <row r="17" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
-      <c r="B17" s="74"/>
+      <c r="B17" s="72"/>
       <c r="C17" s="46" t="s">
         <v>304</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="F17" s="47"/>
     </row>
     <row r="18" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
-      <c r="B18" s="74"/>
+      <c r="B18" s="72"/>
       <c r="C18" s="46" t="s">
         <v>307</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="F18" s="47"/>
     </row>
@@ -12410,45 +12520,45 @@
       <c r="A19" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="B19" s="74" t="s">
+      <c r="B19" s="72" t="s">
         <v>122</v>
       </c>
       <c r="C19" s="46" t="s">
         <v>302</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F19" s="47"/>
     </row>
     <row r="20" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15"/>
-      <c r="B20" s="74"/>
+      <c r="B20" s="72"/>
       <c r="C20" s="46" t="s">
         <v>305</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="F20" s="47"/>
     </row>
     <row r="21" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15"/>
-      <c r="B21" s="74"/>
+      <c r="B21" s="72"/>
       <c r="C21" s="46" t="s">
         <v>308</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="F21" s="47"/>
     </row>
@@ -12456,45 +12566,45 @@
       <c r="A22" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="B22" s="74" t="s">
+      <c r="B22" s="72" t="s">
         <v>123</v>
       </c>
       <c r="C22" s="46" t="s">
         <v>303</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F22" s="47"/>
     </row>
     <row r="23" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15"/>
-      <c r="B23" s="74"/>
+      <c r="B23" s="72"/>
       <c r="C23" s="46" t="s">
         <v>306</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="F23" s="47"/>
     </row>
     <row r="24" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="15"/>
-      <c r="B24" s="74"/>
+      <c r="B24" s="72"/>
       <c r="C24" s="46" t="s">
         <v>303</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="F24" s="47"/>
     </row>
@@ -12502,45 +12612,45 @@
       <c r="A25" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="B25" s="74" t="s">
+      <c r="B25" s="72" t="s">
         <v>124</v>
       </c>
       <c r="C25" s="46" t="s">
         <v>309</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F25" s="47"/>
     </row>
     <row r="26" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="15"/>
-      <c r="B26" s="74"/>
+      <c r="B26" s="72"/>
       <c r="C26" s="46" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="F26" s="47"/>
     </row>
     <row r="27" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="15"/>
-      <c r="B27" s="74"/>
+      <c r="B27" s="72"/>
       <c r="C27" s="46" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="F27" s="47"/>
     </row>
@@ -12548,45 +12658,45 @@
       <c r="A28" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="B28" s="74" t="s">
+      <c r="B28" s="72" t="s">
         <v>125</v>
       </c>
       <c r="C28" s="46" t="s">
         <v>310</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F28" s="47"/>
     </row>
     <row r="29" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="15"/>
-      <c r="B29" s="74"/>
+      <c r="B29" s="72"/>
       <c r="C29" s="46" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="F29" s="47"/>
     </row>
     <row r="30" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="15"/>
-      <c r="B30" s="74"/>
+      <c r="B30" s="72"/>
       <c r="C30" s="46" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="F30" s="47"/>
     </row>
@@ -12594,45 +12704,45 @@
       <c r="A31" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="B31" s="74" t="s">
+      <c r="B31" s="72" t="s">
         <v>126</v>
       </c>
       <c r="C31" s="46" t="s">
         <v>311</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F31" s="47"/>
     </row>
     <row r="32" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="15"/>
-      <c r="B32" s="74"/>
+      <c r="B32" s="72"/>
       <c r="C32" s="46" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="F32" s="47"/>
     </row>
     <row r="33" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="15"/>
-      <c r="B33" s="74"/>
+      <c r="B33" s="72"/>
       <c r="C33" s="46" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="F33" s="47"/>
     </row>
@@ -12640,45 +12750,45 @@
       <c r="A34" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="B34" s="74" t="s">
+      <c r="B34" s="72" t="s">
         <v>127</v>
       </c>
       <c r="C34" s="46" t="s">
         <v>312</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E34" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F34" s="47"/>
     </row>
     <row r="35" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="15"/>
-      <c r="B35" s="74"/>
+      <c r="B35" s="72"/>
       <c r="C35" s="46" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="F35" s="47"/>
     </row>
     <row r="36" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="15"/>
-      <c r="B36" s="74"/>
+      <c r="B36" s="72"/>
       <c r="C36" s="46" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="F36" s="47"/>
     </row>
@@ -12686,45 +12796,45 @@
       <c r="A37" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="B37" s="74" t="s">
+      <c r="B37" s="72" t="s">
         <v>128</v>
       </c>
       <c r="C37" s="46" t="s">
         <v>313</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F37" s="47"/>
     </row>
     <row r="38" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="15"/>
-      <c r="B38" s="74"/>
+      <c r="B38" s="72"/>
       <c r="C38" s="46" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="F38" s="47"/>
     </row>
     <row r="39" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="15"/>
-      <c r="B39" s="74"/>
+      <c r="B39" s="72"/>
       <c r="C39" s="46" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E39" s="18" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="F39" s="47"/>
     </row>
@@ -12732,45 +12842,45 @@
       <c r="A40" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="B40" s="74" t="s">
+      <c r="B40" s="72" t="s">
         <v>129</v>
       </c>
       <c r="C40" s="46" t="s">
         <v>314</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F40" s="47"/>
     </row>
     <row r="41" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="15"/>
-      <c r="B41" s="74"/>
+      <c r="B41" s="72"/>
       <c r="C41" s="46" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="F41" s="47"/>
     </row>
     <row r="42" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="15"/>
-      <c r="B42" s="74"/>
+      <c r="B42" s="72"/>
       <c r="C42" s="46" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E42" s="18" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="F42" s="47"/>
     </row>
@@ -12778,45 +12888,45 @@
       <c r="A43" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="B43" s="74" t="s">
+      <c r="B43" s="72" t="s">
         <v>130</v>
       </c>
       <c r="C43" s="46" t="s">
         <v>315</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E43" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F43" s="47"/>
     </row>
     <row r="44" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="15"/>
-      <c r="B44" s="74"/>
+      <c r="B44" s="72"/>
       <c r="C44" s="46" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E44" s="18" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="F44" s="47"/>
     </row>
     <row r="45" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="15"/>
-      <c r="B45" s="74"/>
+      <c r="B45" s="72"/>
       <c r="C45" s="46" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E45" s="18" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="F45" s="47"/>
     </row>
@@ -12824,45 +12934,45 @@
       <c r="A46" s="40" t="s">
         <v>227</v>
       </c>
-      <c r="B46" s="73" t="s">
+      <c r="B46" s="71" t="s">
         <v>225</v>
       </c>
       <c r="C46" s="44" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D46" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E46" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F46" s="47"/>
     </row>
     <row r="47" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="40"/>
-      <c r="B47" s="73"/>
+      <c r="B47" s="71"/>
       <c r="C47" s="44" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="D47" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E47" s="18" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="F47" s="47"/>
     </row>
     <row r="48" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="40"/>
-      <c r="B48" s="73"/>
+      <c r="B48" s="71"/>
       <c r="C48" s="44" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E48" s="18" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="F48" s="47"/>
     </row>
@@ -12870,45 +12980,45 @@
       <c r="A49" s="40" t="s">
         <v>228</v>
       </c>
-      <c r="B49" s="73" t="s">
+      <c r="B49" s="71" t="s">
         <v>226</v>
       </c>
       <c r="C49" s="44" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D49" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E49" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F49" s="44"/>
     </row>
     <row r="50" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="40"/>
-      <c r="B50" s="73"/>
+      <c r="B50" s="71"/>
       <c r="C50" s="44" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D50" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E50" s="18" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="F50" s="44"/>
     </row>
     <row r="51" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="40"/>
-      <c r="B51" s="73"/>
+      <c r="B51" s="71"/>
       <c r="C51" s="44" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="D51" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E51" s="18" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="F51" s="44"/>
     </row>
@@ -12916,91 +13026,91 @@
       <c r="A52" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="B52" s="74" t="s">
+      <c r="B52" s="72" t="s">
         <v>146</v>
       </c>
       <c r="C52" s="46" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="D52" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E52" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F52" s="44"/>
     </row>
     <row r="53" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="15"/>
-      <c r="B53" s="74"/>
+      <c r="B53" s="72"/>
       <c r="C53" s="46" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="D53" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E53" s="18" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="F53" s="44"/>
     </row>
     <row r="54" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="15"/>
-      <c r="B54" s="74"/>
+      <c r="B54" s="72"/>
       <c r="C54" s="46" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="D54" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E54" s="18" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="F54" s="44"/>
     </row>
     <row r="55" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="40" t="s">
+        <v>352</v>
+      </c>
+      <c r="B55" s="71"/>
+      <c r="C55" s="81" t="s">
+        <v>433</v>
+      </c>
+      <c r="D55" s="18" t="s">
+        <v>413</v>
+      </c>
+      <c r="E55" s="18" t="s">
         <v>353</v>
       </c>
-      <c r="B55" s="73"/>
-      <c r="C55" s="44" t="s">
-        <v>354</v>
-      </c>
-      <c r="D55" s="18" t="s">
-        <v>429</v>
-      </c>
-      <c r="E55" s="18" t="s">
-        <v>429</v>
-      </c>
       <c r="F55" s="44" t="s">
-        <v>430</v>
+        <v>416</v>
       </c>
     </row>
     <row r="56" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="40"/>
-      <c r="B56" s="73"/>
-      <c r="C56" s="44" t="s">
-        <v>355</v>
+      <c r="B56" s="71"/>
+      <c r="C56" s="81" t="s">
+        <v>434</v>
       </c>
       <c r="D56" s="18" t="s">
-        <v>429</v>
+        <v>413</v>
       </c>
       <c r="E56" s="18" t="s">
-        <v>429</v>
+        <v>414</v>
       </c>
       <c r="F56" s="44"/>
     </row>
     <row r="57" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="40"/>
-      <c r="B57" s="73"/>
-      <c r="C57" s="44" t="s">
-        <v>356</v>
+      <c r="B57" s="71"/>
+      <c r="C57" s="81" t="s">
+        <v>435</v>
       </c>
       <c r="D57" s="18" t="s">
-        <v>429</v>
+        <v>413</v>
       </c>
       <c r="E57" s="18" t="s">
-        <v>429</v>
+        <v>415</v>
       </c>
       <c r="F57" s="44"/>
     </row>
@@ -13008,45 +13118,45 @@
       <c r="A58" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="B58" s="73" t="s">
+      <c r="B58" s="71" t="s">
         <v>192</v>
       </c>
       <c r="C58" s="44" t="s">
         <v>341</v>
       </c>
       <c r="D58" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E58" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F58" s="44"/>
     </row>
     <row r="59" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="40"/>
-      <c r="B59" s="73"/>
+      <c r="B59" s="71"/>
       <c r="C59" s="44" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="D59" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E59" s="18" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="F59" s="44"/>
     </row>
     <row r="60" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="40"/>
-      <c r="B60" s="73"/>
+      <c r="B60" s="71"/>
       <c r="C60" s="44" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="D60" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E60" s="18" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="F60" s="44"/>
     </row>
@@ -13054,45 +13164,45 @@
       <c r="A61" s="40" t="s">
         <v>190</v>
       </c>
-      <c r="B61" s="73" t="s">
+      <c r="B61" s="71" t="s">
         <v>193</v>
       </c>
       <c r="C61" s="44" t="s">
         <v>342</v>
       </c>
       <c r="D61" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E61" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F61" s="44"/>
     </row>
     <row r="62" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="40"/>
-      <c r="B62" s="73"/>
+      <c r="B62" s="71"/>
       <c r="C62" s="44" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D62" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E62" s="18" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="F62" s="44"/>
     </row>
     <row r="63" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="40"/>
-      <c r="B63" s="73"/>
+      <c r="B63" s="71"/>
       <c r="C63" s="44" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="D63" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E63" s="18" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="F63" s="44"/>
     </row>
@@ -13100,45 +13210,45 @@
       <c r="A64" s="40" t="s">
         <v>191</v>
       </c>
-      <c r="B64" s="73" t="s">
+      <c r="B64" s="71" t="s">
         <v>194</v>
       </c>
       <c r="C64" s="44" t="s">
         <v>343</v>
       </c>
       <c r="D64" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E64" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F64" s="44"/>
     </row>
     <row r="65" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="40"/>
-      <c r="B65" s="73"/>
+      <c r="B65" s="71"/>
       <c r="C65" s="44" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="D65" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E65" s="18" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="F65" s="44"/>
     </row>
     <row r="66" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="40"/>
-      <c r="B66" s="73"/>
+      <c r="B66" s="71"/>
       <c r="C66" s="44" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="D66" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E66" s="18" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="F66" s="44"/>
     </row>
@@ -13146,45 +13256,45 @@
       <c r="A67" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="B67" s="73" t="s">
+      <c r="B67" s="71" t="s">
         <v>223</v>
       </c>
       <c r="C67" s="44" t="s">
         <v>344</v>
       </c>
       <c r="D67" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E67" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F67" s="44"/>
     </row>
     <row r="68" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="40"/>
-      <c r="B68" s="73"/>
+      <c r="B68" s="71"/>
       <c r="C68" s="44" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="D68" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E68" s="18" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="F68" s="44"/>
     </row>
     <row r="69" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="40"/>
-      <c r="B69" s="73"/>
+      <c r="B69" s="71"/>
       <c r="C69" s="44" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D69" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E69" s="18" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="F69" s="44"/>
     </row>
@@ -13192,31 +13302,33 @@
       <c r="A70" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B70" s="74"/>
-      <c r="C70" s="46"/>
+      <c r="B70" s="72"/>
+      <c r="C70" s="82" t="s">
+        <v>438</v>
+      </c>
       <c r="D70" s="18" t="s">
-        <v>433</v>
+        <v>419</v>
       </c>
       <c r="E70" s="18" t="s">
-        <v>438</v>
+        <v>424</v>
       </c>
       <c r="F70" s="47" t="s">
-        <v>437</v>
+        <v>423</v>
       </c>
     </row>
     <row r="71" spans="1:6" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B71" s="74"/>
+      <c r="B71" s="72"/>
       <c r="C71" s="46" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="D71" s="18" t="s">
-        <v>433</v>
+        <v>419</v>
       </c>
       <c r="E71" s="18" t="s">
-        <v>438</v>
+        <v>424</v>
       </c>
       <c r="F71" s="47" t="s">
         <v>101</v>
@@ -13226,169 +13338,171 @@
       <c r="A72" s="40" t="s">
         <v>275</v>
       </c>
-      <c r="B72" s="73" t="s">
+      <c r="B72" s="71" t="s">
         <v>288</v>
       </c>
       <c r="C72" s="44" t="s">
-        <v>402</v>
+        <v>440</v>
       </c>
       <c r="D72" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E72" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F72" s="47" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="73" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="40"/>
-      <c r="B73" s="73"/>
+      <c r="B73" s="71"/>
       <c r="C73" s="44" t="s">
-        <v>403</v>
+        <v>441</v>
       </c>
       <c r="D73" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E73" s="18" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="F73" s="47" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="40"/>
-      <c r="B74" s="73"/>
+      <c r="B74" s="71"/>
       <c r="C74" s="44" t="s">
-        <v>404</v>
+        <v>442</v>
       </c>
       <c r="D74" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E74" s="18" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="F74" s="47" t="s">
-        <v>446</v>
+        <v>432</v>
       </c>
     </row>
     <row r="75" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="40" t="s">
         <v>276</v>
       </c>
-      <c r="B75" s="73" t="s">
+      <c r="B75" s="71" t="s">
         <v>289</v>
       </c>
       <c r="C75" s="44" t="s">
-        <v>405</v>
+        <v>443</v>
       </c>
       <c r="D75" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E75" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F75" s="47" t="s">
-        <v>446</v>
+        <v>432</v>
       </c>
     </row>
     <row r="76" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="40"/>
-      <c r="B76" s="73"/>
+      <c r="B76" s="71"/>
       <c r="C76" s="44" t="s">
-        <v>406</v>
+        <v>444</v>
       </c>
       <c r="D76" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E76" s="18" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="F76" s="47" t="s">
-        <v>446</v>
+        <v>432</v>
       </c>
     </row>
     <row r="77" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="40"/>
-      <c r="B77" s="73"/>
+      <c r="B77" s="71"/>
       <c r="C77" s="44" t="s">
-        <v>407</v>
+        <v>445</v>
       </c>
       <c r="D77" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E77" s="18" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="F77" s="47" t="s">
-        <v>446</v>
+        <v>432</v>
       </c>
     </row>
     <row r="78" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="40" t="s">
         <v>277</v>
       </c>
-      <c r="B78" s="73" t="s">
+      <c r="B78" s="71" t="s">
         <v>290</v>
       </c>
       <c r="C78" s="44" t="s">
-        <v>395</v>
+        <v>446</v>
       </c>
       <c r="D78" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E78" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F78" s="47" t="s">
-        <v>446</v>
+        <v>432</v>
       </c>
     </row>
     <row r="79" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="40"/>
-      <c r="B79" s="73"/>
+      <c r="B79" s="71"/>
       <c r="C79" s="44" t="s">
-        <v>396</v>
+        <v>447</v>
       </c>
       <c r="D79" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E79" s="18" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="F79" s="47" t="s">
-        <v>446</v>
+        <v>432</v>
       </c>
     </row>
     <row r="80" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="40"/>
-      <c r="B80" s="73"/>
+      <c r="B80" s="71"/>
       <c r="C80" s="44" t="s">
-        <v>397</v>
+        <v>448</v>
       </c>
       <c r="D80" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E80" s="18" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="F80" s="47" t="s">
-        <v>446</v>
+        <v>432</v>
       </c>
     </row>
     <row r="81" spans="1:8" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A81" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B81" s="74"/>
-      <c r="C81" s="46"/>
+      <c r="B81" s="72"/>
+      <c r="C81" s="82" t="s">
+        <v>439</v>
+      </c>
       <c r="D81" s="18" t="s">
-        <v>433</v>
+        <v>419</v>
       </c>
       <c r="E81" s="18" t="s">
-        <v>438</v>
+        <v>424</v>
       </c>
       <c r="F81" s="47" t="s">
         <v>37</v>
@@ -13398,15 +13512,15 @@
       <c r="A82" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B82" s="74"/>
+      <c r="B82" s="72"/>
       <c r="C82" s="46" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="D82" s="18" t="s">
-        <v>433</v>
+        <v>419</v>
       </c>
       <c r="E82" s="18" t="s">
-        <v>438</v>
+        <v>424</v>
       </c>
       <c r="F82" s="47" t="s">
         <v>38</v>
@@ -13416,17 +13530,17 @@
       <c r="A83" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="B83" s="74" t="s">
+      <c r="B83" s="72" t="s">
         <v>291</v>
       </c>
       <c r="C83" s="46" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="D83" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E83" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F83" s="47" t="s">
         <v>278</v>
@@ -13436,13 +13550,15 @@
     </row>
     <row r="84" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="15"/>
-      <c r="B84" s="74"/>
-      <c r="C84" s="46"/>
+      <c r="B84" s="72"/>
+      <c r="C84" s="46" t="s">
+        <v>449</v>
+      </c>
       <c r="D84" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E84" s="18" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="F84" s="47"/>
       <c r="G84" s="12"/>
@@ -13450,13 +13566,15 @@
     </row>
     <row r="85" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="15"/>
-      <c r="B85" s="74"/>
-      <c r="C85" s="46"/>
+      <c r="B85" s="72"/>
+      <c r="C85" s="46" t="s">
+        <v>450</v>
+      </c>
       <c r="D85" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E85" s="18" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="F85" s="47"/>
       <c r="G85" s="12"/>
@@ -13466,33 +13584,35 @@
       <c r="A86" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="B86" s="74" t="s">
+      <c r="B86" s="72" t="s">
         <v>280</v>
       </c>
       <c r="C86" s="46" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="D86" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E86" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F86" s="15" t="s">
-        <v>443</v>
+        <v>429</v>
       </c>
       <c r="G86" s="12"/>
       <c r="H86" s="12"/>
     </row>
     <row r="87" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="15"/>
-      <c r="B87" s="74"/>
-      <c r="C87" s="46"/>
+      <c r="B87" s="72"/>
+      <c r="C87" s="46" t="s">
+        <v>451</v>
+      </c>
       <c r="D87" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E87" s="18" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="F87" s="12"/>
       <c r="G87" s="12"/>
@@ -13500,13 +13620,15 @@
     </row>
     <row r="88" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="15"/>
-      <c r="B88" s="74"/>
-      <c r="C88" s="46"/>
+      <c r="B88" s="72"/>
+      <c r="C88" s="46" t="s">
+        <v>452</v>
+      </c>
       <c r="D88" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E88" s="18" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="F88" s="12"/>
       <c r="G88" s="12"/>
@@ -13516,17 +13638,17 @@
       <c r="A89" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="B89" s="74" t="s">
+      <c r="B89" s="72" t="s">
         <v>124</v>
       </c>
       <c r="C89" s="46" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="D89" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E89" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F89" s="12" t="s">
         <v>279</v>
@@ -13536,13 +13658,15 @@
     </row>
     <row r="90" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="15"/>
-      <c r="B90" s="74"/>
-      <c r="C90" s="46"/>
+      <c r="B90" s="72"/>
+      <c r="C90" s="46" t="s">
+        <v>453</v>
+      </c>
       <c r="D90" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E90" s="18" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="F90" s="12"/>
       <c r="G90" s="12"/>
@@ -13550,13 +13674,15 @@
     </row>
     <row r="91" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="15"/>
-      <c r="B91" s="74"/>
-      <c r="C91" s="46"/>
+      <c r="B91" s="72"/>
+      <c r="C91" s="46" t="s">
+        <v>454</v>
+      </c>
       <c r="D91" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E91" s="18" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="F91" s="12"/>
       <c r="G91" s="12"/>
@@ -13566,33 +13692,35 @@
       <c r="A92" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="B92" s="74" t="s">
+      <c r="B92" s="72" t="s">
         <v>281</v>
       </c>
-      <c r="C92" s="46" t="s">
-        <v>408</v>
+      <c r="C92" s="83" t="s">
+        <v>395</v>
       </c>
       <c r="D92" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E92" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F92" s="15" t="s">
-        <v>443</v>
+        <v>429</v>
       </c>
       <c r="G92" s="12"/>
       <c r="H92" s="12"/>
     </row>
     <row r="93" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="15"/>
-      <c r="B93" s="74"/>
-      <c r="C93" s="46"/>
+      <c r="B93" s="72"/>
+      <c r="C93" s="83" t="s">
+        <v>455</v>
+      </c>
       <c r="D93" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E93" s="18" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="F93" s="12"/>
       <c r="G93" s="12"/>
@@ -13600,13 +13728,15 @@
     </row>
     <row r="94" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="15"/>
-      <c r="B94" s="74"/>
-      <c r="C94" s="46"/>
+      <c r="B94" s="72"/>
+      <c r="C94" s="83" t="s">
+        <v>456</v>
+      </c>
       <c r="D94" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E94" s="18" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="F94" s="12"/>
       <c r="G94" s="12"/>
@@ -13616,17 +13746,17 @@
       <c r="A95" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="B95" s="74" t="s">
+      <c r="B95" s="72" t="s">
         <v>130</v>
       </c>
       <c r="C95" s="46" t="s">
-        <v>409</v>
+        <v>396</v>
       </c>
       <c r="D95" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E95" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F95" s="12" t="s">
         <v>279</v>
@@ -13636,13 +13766,15 @@
     </row>
     <row r="96" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="15"/>
-      <c r="B96" s="74"/>
-      <c r="C96" s="46"/>
+      <c r="B96" s="72"/>
+      <c r="C96" s="46" t="s">
+        <v>457</v>
+      </c>
       <c r="D96" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E96" s="18" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="F96" s="12"/>
       <c r="G96" s="12"/>
@@ -13650,13 +13782,15 @@
     </row>
     <row r="97" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="15"/>
-      <c r="B97" s="74"/>
-      <c r="C97" s="46"/>
+      <c r="B97" s="72"/>
+      <c r="C97" s="46" t="s">
+        <v>458</v>
+      </c>
       <c r="D97" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E97" s="18" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="F97" s="12"/>
       <c r="G97" s="12"/>
@@ -13666,33 +13800,35 @@
       <c r="A98" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="B98" s="74" t="s">
+      <c r="B98" s="72" t="s">
         <v>282</v>
       </c>
       <c r="C98" s="46" t="s">
-        <v>410</v>
+        <v>397</v>
       </c>
       <c r="D98" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E98" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F98" s="15" t="s">
-        <v>443</v>
+        <v>429</v>
       </c>
       <c r="G98" s="12"/>
       <c r="H98" s="12"/>
     </row>
     <row r="99" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="15"/>
-      <c r="B99" s="74"/>
-      <c r="C99" s="46"/>
+      <c r="B99" s="72"/>
+      <c r="C99" s="46" t="s">
+        <v>459</v>
+      </c>
       <c r="D99" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E99" s="18" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="F99" s="12"/>
       <c r="G99" s="12"/>
@@ -13700,13 +13836,15 @@
     </row>
     <row r="100" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="15"/>
-      <c r="B100" s="74"/>
-      <c r="C100" s="46"/>
+      <c r="B100" s="72"/>
+      <c r="C100" s="46" t="s">
+        <v>460</v>
+      </c>
       <c r="D100" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E100" s="18" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="F100" s="12"/>
       <c r="G100" s="12"/>
@@ -13716,17 +13854,17 @@
       <c r="A101" s="15" t="s">
         <v>283</v>
       </c>
-      <c r="B101" s="74" t="s">
+      <c r="B101" s="72" t="s">
         <v>290</v>
       </c>
       <c r="C101" s="46" t="s">
-        <v>411</v>
+        <v>398</v>
       </c>
       <c r="D101" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E101" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F101" s="12" t="s">
         <v>279</v>
@@ -13736,13 +13874,15 @@
     </row>
     <row r="102" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="15"/>
-      <c r="B102" s="74"/>
-      <c r="C102" s="46"/>
+      <c r="B102" s="72"/>
+      <c r="C102" s="46" t="s">
+        <v>461</v>
+      </c>
       <c r="D102" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E102" s="18" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="F102" s="12"/>
       <c r="G102" s="12"/>
@@ -13750,13 +13890,15 @@
     </row>
     <row r="103" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="15"/>
-      <c r="B103" s="74"/>
-      <c r="C103" s="46"/>
+      <c r="B103" s="72"/>
+      <c r="C103" s="46" t="s">
+        <v>462</v>
+      </c>
       <c r="D103" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E103" s="18" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="F103" s="12"/>
       <c r="G103" s="12"/>
@@ -13766,33 +13908,35 @@
       <c r="A104" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="B104" s="74" t="s">
+      <c r="B104" s="72" t="s">
         <v>285</v>
       </c>
       <c r="C104" s="46" t="s">
-        <v>412</v>
+        <v>399</v>
       </c>
       <c r="D104" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E104" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F104" s="15" t="s">
-        <v>443</v>
+        <v>429</v>
       </c>
       <c r="G104" s="12"/>
       <c r="H104" s="12"/>
     </row>
     <row r="105" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="15"/>
-      <c r="B105" s="74"/>
-      <c r="C105" s="46"/>
+      <c r="B105" s="72"/>
+      <c r="C105" s="46" t="s">
+        <v>463</v>
+      </c>
       <c r="D105" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E105" s="18" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="F105" s="47"/>
       <c r="G105" s="12"/>
@@ -13800,19 +13944,21 @@
     </row>
     <row r="106" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="40"/>
-      <c r="B106" s="73"/>
-      <c r="C106" s="44"/>
+      <c r="B106" s="71"/>
+      <c r="C106" s="44" t="s">
+        <v>464</v>
+      </c>
       <c r="D106" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E106" s="18" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="F106" s="44"/>
     </row>
     <row r="107" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="40"/>
-      <c r="B107" s="73"/>
+      <c r="B107" s="71"/>
       <c r="C107" s="44"/>
       <c r="D107" s="18"/>
       <c r="E107" s="18"/>
@@ -13822,59 +13968,67 @@
       <c r="A108" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="B108" s="74"/>
-      <c r="C108" s="45"/>
+      <c r="B108" s="72"/>
+      <c r="C108" s="45" t="s">
+        <v>465</v>
+      </c>
       <c r="D108" s="41" t="s">
-        <v>433</v>
+        <v>419</v>
       </c>
       <c r="E108" s="41" t="s">
-        <v>439</v>
+        <v>425</v>
       </c>
       <c r="F108" s="44" t="s">
-        <v>440</v>
+        <v>426</v>
       </c>
     </row>
     <row r="109" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="40" t="s">
-        <v>94</v>
-      </c>
-      <c r="B109" s="74"/>
-      <c r="C109" s="45"/>
+        <v>95</v>
+      </c>
+      <c r="B109" s="72"/>
+      <c r="C109" s="45" t="s">
+        <v>467</v>
+      </c>
       <c r="D109" s="41" t="s">
-        <v>433</v>
+        <v>419</v>
       </c>
       <c r="E109" s="41" t="s">
-        <v>439</v>
-      </c>
-      <c r="F109" s="44"/>
+        <v>425</v>
+      </c>
+      <c r="F109" s="44" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="110" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="40" t="s">
-        <v>95</v>
-      </c>
-      <c r="B110" s="74"/>
-      <c r="C110" s="45"/>
+        <v>94</v>
+      </c>
+      <c r="B110" s="72"/>
+      <c r="C110" s="45" t="s">
+        <v>466</v>
+      </c>
       <c r="D110" s="41" t="s">
-        <v>433</v>
+        <v>419</v>
       </c>
       <c r="E110" s="41" t="s">
-        <v>439</v>
-      </c>
-      <c r="F110" s="44" t="s">
-        <v>434</v>
-      </c>
+        <v>425</v>
+      </c>
+      <c r="F110" s="44"/>
     </row>
     <row r="111" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="B111" s="74"/>
-      <c r="C111" s="45"/>
+      <c r="B111" s="72"/>
+      <c r="C111" s="45" t="s">
+        <v>468</v>
+      </c>
       <c r="D111" s="41" t="s">
-        <v>433</v>
+        <v>419</v>
       </c>
       <c r="E111" s="41" t="s">
-        <v>439</v>
+        <v>425</v>
       </c>
       <c r="F111" s="44"/>
     </row>
@@ -13882,13 +14036,15 @@
       <c r="A112" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="B112" s="74"/>
-      <c r="C112" s="45"/>
+      <c r="B112" s="72"/>
+      <c r="C112" s="45" t="s">
+        <v>469</v>
+      </c>
       <c r="D112" s="41" t="s">
-        <v>433</v>
+        <v>419</v>
       </c>
       <c r="E112" s="41" t="s">
-        <v>433</v>
+        <v>419</v>
       </c>
       <c r="F112" s="44"/>
     </row>
@@ -13897,13 +14053,15 @@
       <c r="A114" t="s">
         <v>98</v>
       </c>
-      <c r="B114" s="74"/>
-      <c r="C114" s="46"/>
+      <c r="B114" s="72"/>
+      <c r="C114" s="80" t="s">
+        <v>470</v>
+      </c>
       <c r="D114" s="18" t="s">
-        <v>432</v>
+        <v>418</v>
       </c>
       <c r="E114" s="18" t="s">
-        <v>432</v>
+        <v>418</v>
       </c>
       <c r="F114" s="47" t="s">
         <v>348</v>
@@ -13913,77 +14071,81 @@
       <c r="A115" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="B115" s="75" t="s">
+      <c r="B115" s="73" t="s">
         <v>99</v>
       </c>
       <c r="C115" t="s">
         <v>345</v>
       </c>
       <c r="D115" s="41" t="s">
-        <v>433</v>
+        <v>419</v>
       </c>
       <c r="E115" s="41" t="s">
         <v>347</v>
       </c>
       <c r="F115" s="47" t="s">
-        <v>442</v>
+        <v>428</v>
       </c>
     </row>
     <row r="116" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="B116" s="75" t="s">
+      <c r="B116" s="73" t="s">
         <v>100</v>
       </c>
       <c r="C116" t="s">
         <v>346</v>
       </c>
       <c r="D116" s="41" t="s">
-        <v>433</v>
+        <v>419</v>
       </c>
       <c r="E116" s="41" t="s">
         <v>347</v>
       </c>
       <c r="F116" s="47" t="s">
-        <v>442</v>
+        <v>428</v>
       </c>
     </row>
     <row r="117" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A117" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B117" s="75"/>
-      <c r="C117"/>
+      <c r="B117" s="73"/>
+      <c r="C117" t="s">
+        <v>471</v>
+      </c>
       <c r="D117" s="41" t="s">
-        <v>433</v>
+        <v>419</v>
       </c>
       <c r="E117" s="41" t="s">
         <v>347</v>
       </c>
       <c r="F117" s="47" t="s">
-        <v>444</v>
+        <v>430</v>
       </c>
     </row>
     <row r="118" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="B118" s="74"/>
-      <c r="C118" s="46"/>
+      <c r="B118" s="72"/>
+      <c r="C118" s="46" t="s">
+        <v>472</v>
+      </c>
       <c r="D118" s="41" t="s">
-        <v>433</v>
+        <v>419</v>
       </c>
       <c r="E118" s="41" t="s">
         <v>347</v>
       </c>
       <c r="F118" s="47" t="s">
-        <v>444</v>
+        <v>430</v>
       </c>
     </row>
     <row r="119" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="15"/>
-      <c r="B119" s="74"/>
+      <c r="B119" s="72"/>
       <c r="C119" s="46"/>
       <c r="D119" s="18"/>
       <c r="E119" s="18"/>
@@ -13993,21 +14155,23 @@
       <c r="A120" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B120" s="74"/>
-      <c r="C120" s="46"/>
+      <c r="B120" s="72"/>
+      <c r="C120" s="46" t="s">
+        <v>473</v>
+      </c>
       <c r="D120" s="18" t="s">
-        <v>432</v>
+        <v>418</v>
       </c>
       <c r="E120" s="18" t="s">
-        <v>432</v>
+        <v>418</v>
       </c>
       <c r="F120" s="47" t="s">
-        <v>445</v>
+        <v>431</v>
       </c>
     </row>
     <row r="121" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="15"/>
-      <c r="B121" s="74"/>
+      <c r="B121" s="72"/>
       <c r="C121" s="46"/>
       <c r="D121" s="18"/>
       <c r="E121" s="18"/>
@@ -14015,17 +14179,17 @@
     </row>
     <row r="122" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="15" t="s">
-        <v>413</v>
-      </c>
-      <c r="B122" s="74"/>
+        <v>400</v>
+      </c>
+      <c r="B122" s="72"/>
       <c r="C122" s="46" t="s">
-        <v>414</v>
+        <v>401</v>
       </c>
       <c r="D122" s="18" t="s">
-        <v>432</v>
+        <v>418</v>
       </c>
       <c r="E122" s="18" t="s">
-        <v>432</v>
+        <v>418</v>
       </c>
       <c r="F122" s="47"/>
     </row>
@@ -14033,15 +14197,15 @@
       <c r="A123" s="15" t="s">
         <v>319</v>
       </c>
-      <c r="B123" s="74"/>
+      <c r="B123" s="72"/>
       <c r="C123" s="46" t="s">
         <v>318</v>
       </c>
       <c r="D123" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E123" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F123" s="47" t="s">
         <v>316</v>
@@ -14051,15 +14215,15 @@
       <c r="A124" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="B124" s="74"/>
+      <c r="B124" s="72"/>
       <c r="C124" s="46" t="s">
         <v>322</v>
       </c>
       <c r="D124" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E124" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F124" s="47"/>
     </row>
@@ -14067,15 +14231,15 @@
       <c r="A125" s="15" t="s">
         <v>321</v>
       </c>
-      <c r="B125" s="74"/>
+      <c r="B125" s="72"/>
       <c r="C125" s="46" t="s">
         <v>323</v>
       </c>
       <c r="D125" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E125" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F125" s="47"/>
     </row>
@@ -14083,31 +14247,31 @@
       <c r="A126" s="15" t="s">
         <v>317</v>
       </c>
-      <c r="B126" s="74"/>
+      <c r="B126" s="72"/>
       <c r="C126" s="46" t="s">
         <v>324</v>
       </c>
       <c r="D126" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E126" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F126" s="47"/>
     </row>
     <row r="127" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="15" t="s">
-        <v>415</v>
-      </c>
-      <c r="B127" s="74"/>
+        <v>402</v>
+      </c>
+      <c r="B127" s="72"/>
       <c r="C127" s="46" t="s">
-        <v>416</v>
+        <v>403</v>
       </c>
       <c r="D127" s="18" t="s">
-        <v>432</v>
+        <v>418</v>
       </c>
       <c r="E127" s="18" t="s">
-        <v>432</v>
+        <v>418</v>
       </c>
       <c r="F127" s="47"/>
     </row>
@@ -14115,82 +14279,82 @@
       <c r="A128" s="15" t="s">
         <v>325</v>
       </c>
-      <c r="B128" s="74"/>
+      <c r="B128" s="72"/>
       <c r="C128" s="46" t="s">
         <v>340</v>
       </c>
       <c r="D128" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E128" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F128" s="47" t="s">
-        <v>441</v>
+        <v>427</v>
       </c>
     </row>
     <row r="129" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="15" t="s">
         <v>326</v>
       </c>
-      <c r="B129" s="74"/>
+      <c r="B129" s="72"/>
       <c r="C129" s="46" t="s">
         <v>339</v>
       </c>
       <c r="D129" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E129" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="130" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A130" s="15" t="s">
         <v>327</v>
       </c>
-      <c r="B130" s="74"/>
+      <c r="B130" s="72"/>
       <c r="C130" s="46" t="s">
         <v>338</v>
       </c>
       <c r="D130" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E130" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F130" s="15" t="s">
-        <v>419</v>
+        <v>406</v>
       </c>
     </row>
     <row r="131" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="15" t="s">
         <v>328</v>
       </c>
-      <c r="B131" s="74"/>
+      <c r="B131" s="72"/>
       <c r="C131" s="46" t="s">
         <v>337</v>
       </c>
       <c r="D131" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E131" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F131" s="47"/>
     </row>
     <row r="132" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="15" t="s">
-        <v>417</v>
-      </c>
-      <c r="B132" s="74"/>
+        <v>404</v>
+      </c>
+      <c r="B132" s="72"/>
       <c r="C132" s="46" t="s">
+        <v>405</v>
+      </c>
+      <c r="D132" s="18" t="s">
         <v>418</v>
       </c>
-      <c r="D132" s="18" t="s">
-        <v>432</v>
-      </c>
       <c r="E132" s="18" t="s">
-        <v>432</v>
+        <v>418</v>
       </c>
       <c r="F132" s="47"/>
     </row>
@@ -14198,15 +14362,15 @@
       <c r="A133" s="15" t="s">
         <v>329</v>
       </c>
-      <c r="B133" s="74"/>
+      <c r="B133" s="72"/>
       <c r="C133" s="46" t="s">
         <v>336</v>
       </c>
       <c r="D133" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E133" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F133" s="47"/>
     </row>
@@ -14214,15 +14378,15 @@
       <c r="A134" s="15" t="s">
         <v>330</v>
       </c>
-      <c r="B134" s="74"/>
+      <c r="B134" s="72"/>
       <c r="C134" s="46" t="s">
         <v>335</v>
       </c>
       <c r="D134" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E134" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F134" s="47"/>
     </row>
@@ -14230,15 +14394,15 @@
       <c r="A135" s="15" t="s">
         <v>331</v>
       </c>
-      <c r="B135" s="74"/>
+      <c r="B135" s="72"/>
       <c r="C135" s="46" t="s">
         <v>334</v>
       </c>
       <c r="D135" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E135" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F135" s="47"/>
     </row>
@@ -14246,28 +14410,28 @@
       <c r="A136" s="15" t="s">
         <v>332</v>
       </c>
-      <c r="B136" s="74"/>
+      <c r="B136" s="72"/>
       <c r="C136" s="46" t="s">
         <v>333</v>
       </c>
       <c r="D136" s="18" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="E136" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F136" s="47"/>
     </row>
     <row r="137" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="15"/>
-      <c r="B137" s="74"/>
+      <c r="B137" s="72"/>
       <c r="C137" s="46"/>
       <c r="D137" s="18"/>
       <c r="E137" s="18"/>
       <c r="F137" s="47"/>
     </row>
     <row r="138" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B138" s="74"/>
+      <c r="B138" s="72"/>
       <c r="C138" s="46"/>
       <c r="D138" s="18"/>
       <c r="E138" s="18"/>
@@ -14322,10 +14486,10 @@
       <c r="F144" s="47"/>
     </row>
     <row r="145" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="78" t="s">
-        <v>420</v>
-      </c>
-      <c r="B145" s="79">
+      <c r="A145" s="76" t="s">
+        <v>407</v>
+      </c>
+      <c r="B145" s="77">
         <f>(B146*B147*1440*B148) / 10000000</f>
         <v>3.024</v>
       </c>
@@ -14335,10 +14499,10 @@
       <c r="F145" s="47"/>
     </row>
     <row r="146" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="76" t="s">
-        <v>421</v>
-      </c>
-      <c r="B146" s="77">
+      <c r="A146" s="74" t="s">
+        <v>408</v>
+      </c>
+      <c r="B146" s="75">
         <v>150</v>
       </c>
       <c r="C146" s="46"/>
@@ -14347,10 +14511,10 @@
       <c r="F146" s="47"/>
     </row>
     <row r="147" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="76" t="s">
-        <v>422</v>
-      </c>
-      <c r="B147" s="77">
+      <c r="A147" s="74" t="s">
+        <v>409</v>
+      </c>
+      <c r="B147" s="75">
         <v>7</v>
       </c>
       <c r="C147" s="46"/>
@@ -14359,10 +14523,10 @@
       <c r="F147" s="47"/>
     </row>
     <row r="148" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="76" t="s">
-        <v>423</v>
-      </c>
-      <c r="B148" s="77">
+      <c r="A148" s="74" t="s">
+        <v>410</v>
+      </c>
+      <c r="B148" s="75">
         <v>20</v>
       </c>
       <c r="C148" s="46"/>
@@ -15492,7 +15656,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="69" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -15503,16 +15667,16 @@
         <v>118</v>
       </c>
       <c r="C3" s="68" t="s">
+        <v>354</v>
+      </c>
+      <c r="D3" s="68" t="s">
+        <v>355</v>
+      </c>
+      <c r="E3" s="68" t="s">
+        <v>356</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>358</v>
-      </c>
-      <c r="D3" s="68" t="s">
-        <v>359</v>
-      </c>
-      <c r="E3" s="68" t="s">
-        <v>360</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>362</v>
       </c>
       <c r="G3" s="11" t="s">
         <v>349</v>

</xml_diff>

<commit_message>
Changed data output file to exclude xbee battery data
Instead, added them to a LoggerLib.py diagParams list
</commit_message>
<xml_diff>
--- a/CombSpillageCode.xlsx
+++ b/CombSpillageCode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sampling sequence" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2121" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2127" uniqueCount="480">
   <si>
     <t>Second</t>
   </si>
@@ -1477,6 +1477,24 @@
   </si>
   <si>
     <t>sec_count</t>
+  </si>
+  <si>
+    <t>vbatt_x005F_xbee1_min</t>
+  </si>
+  <si>
+    <t>vbatt_x005F_xbee1_max</t>
+  </si>
+  <si>
+    <t>vbatt_x005F_xbee2_min</t>
+  </si>
+  <si>
+    <t>vbatt_x005F_xbee2_max</t>
+  </si>
+  <si>
+    <t>vbatt_x005F_xbee3_min</t>
+  </si>
+  <si>
+    <t>vbatt_x005F_xbee3_max</t>
   </si>
 </sst>
 </file>
@@ -1916,12 +1934,6 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1933,6 +1945,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2418,18 +2436,18 @@
       <c r="D4" s="51"/>
       <c r="E4" s="51"/>
       <c r="F4" s="51"/>
-      <c r="G4" s="78" t="s">
+      <c r="G4" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="78"/>
+      <c r="H4" s="82"/>
+      <c r="I4" s="82"/>
+      <c r="J4" s="82"/>
       <c r="K4" s="51"/>
-      <c r="L4" s="78" t="s">
+      <c r="L4" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="78"/>
-      <c r="N4" s="78"/>
+      <c r="M4" s="82"/>
+      <c r="N4" s="82"/>
       <c r="O4" s="51"/>
       <c r="P4" s="51"/>
       <c r="R4" s="7"/>
@@ -2438,10 +2456,10 @@
       <c r="U4" s="7"/>
       <c r="V4" s="7"/>
       <c r="W4" s="7"/>
-      <c r="X4" s="79" t="s">
+      <c r="X4" s="83" t="s">
         <v>53</v>
       </c>
-      <c r="Y4" s="79"/>
+      <c r="Y4" s="83"/>
       <c r="Z4" s="7"/>
       <c r="AA4" s="7"/>
       <c r="AB4" s="7"/>
@@ -2453,10 +2471,10 @@
       <c r="AH4" s="7"/>
       <c r="AI4" s="7"/>
       <c r="AJ4" s="7"/>
-      <c r="AK4" s="79" t="s">
+      <c r="AK4" s="83" t="s">
         <v>53</v>
       </c>
-      <c r="AL4" s="79"/>
+      <c r="AL4" s="83"/>
       <c r="AM4" s="7"/>
       <c r="AN4" s="7"/>
       <c r="AO4" s="7"/>
@@ -12262,12 +12280,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H328"/>
+  <dimension ref="A1:H321"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A119" activePane="bottomLeft" state="frozenSplit"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A114" activePane="bottomLeft" state="frozenSplit"/>
       <selection sqref="A1:A1048576"/>
-      <selection pane="bottomLeft" activeCell="C136" sqref="C136"/>
+      <selection pane="bottomLeft" activeCell="C133" sqref="C133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12370,29 +12388,35 @@
         <v>351</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="40"/>
-      <c r="B9" s="71"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="44"/>
+    <row r="9" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="B9" s="72" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" s="46" t="s">
+        <v>295</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>413</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="F9" s="47"/>
     </row>
     <row r="10" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="B10" s="72" t="s">
-        <v>119</v>
-      </c>
+      <c r="A10" s="15"/>
+      <c r="B10" s="72"/>
       <c r="C10" s="46" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D10" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>353</v>
+        <v>414</v>
       </c>
       <c r="F10" s="47"/>
     </row>
@@ -12400,45 +12424,45 @@
       <c r="A11" s="15"/>
       <c r="B11" s="72"/>
       <c r="C11" s="46" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D11" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F11" s="47"/>
     </row>
     <row r="12" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="72"/>
+      <c r="A12" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" s="72" t="s">
+        <v>120</v>
+      </c>
       <c r="C12" s="46" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D12" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>415</v>
+        <v>353</v>
       </c>
       <c r="F12" s="47"/>
     </row>
     <row r="13" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="B13" s="72" t="s">
-        <v>120</v>
-      </c>
+      <c r="A13" s="15"/>
+      <c r="B13" s="72"/>
       <c r="C13" s="46" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D13" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>353</v>
+        <v>414</v>
       </c>
       <c r="F13" s="47"/>
     </row>
@@ -12446,45 +12470,45 @@
       <c r="A14" s="15"/>
       <c r="B14" s="72"/>
       <c r="C14" s="46" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D14" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F14" s="47"/>
     </row>
     <row r="15" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="B15" s="72"/>
+      <c r="A15" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="72" t="s">
+        <v>121</v>
+      </c>
       <c r="C15" s="46" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D15" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>415</v>
+        <v>353</v>
       </c>
       <c r="F15" s="47"/>
     </row>
     <row r="16" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="B16" s="72" t="s">
-        <v>121</v>
-      </c>
+      <c r="A16" s="15"/>
+      <c r="B16" s="72"/>
       <c r="C16" s="46" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>353</v>
+        <v>414</v>
       </c>
       <c r="F16" s="47"/>
     </row>
@@ -12492,45 +12516,45 @@
       <c r="A17" s="15"/>
       <c r="B17" s="72"/>
       <c r="C17" s="46" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="D17" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F17" s="47"/>
     </row>
     <row r="18" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="72"/>
+      <c r="A18" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B18" s="72" t="s">
+        <v>122</v>
+      </c>
       <c r="C18" s="46" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="D18" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>415</v>
+        <v>353</v>
       </c>
       <c r="F18" s="47"/>
     </row>
     <row r="19" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="B19" s="72" t="s">
-        <v>122</v>
-      </c>
+      <c r="A19" s="15"/>
+      <c r="B19" s="72"/>
       <c r="C19" s="46" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="D19" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>353</v>
+        <v>414</v>
       </c>
       <c r="F19" s="47"/>
     </row>
@@ -12538,45 +12562,45 @@
       <c r="A20" s="15"/>
       <c r="B20" s="72"/>
       <c r="C20" s="46" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="D20" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F20" s="47"/>
     </row>
     <row r="21" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
-      <c r="B21" s="72"/>
+      <c r="A21" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B21" s="72" t="s">
+        <v>123</v>
+      </c>
       <c r="C21" s="46" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D21" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>415</v>
+        <v>353</v>
       </c>
       <c r="F21" s="47"/>
     </row>
     <row r="22" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="B22" s="72" t="s">
-        <v>123</v>
-      </c>
+      <c r="A22" s="15"/>
+      <c r="B22" s="72"/>
       <c r="C22" s="46" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="D22" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>353</v>
+        <v>414</v>
       </c>
       <c r="F22" s="47"/>
     </row>
@@ -12584,45 +12608,45 @@
       <c r="A23" s="15"/>
       <c r="B23" s="72"/>
       <c r="C23" s="46" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D23" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F23" s="47"/>
     </row>
     <row r="24" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
-      <c r="B24" s="72"/>
+      <c r="A24" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="B24" s="72" t="s">
+        <v>124</v>
+      </c>
       <c r="C24" s="46" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
       <c r="D24" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>415</v>
+        <v>353</v>
       </c>
       <c r="F24" s="47"/>
     </row>
     <row r="25" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="B25" s="72" t="s">
-        <v>124</v>
-      </c>
+      <c r="A25" s="15"/>
+      <c r="B25" s="72"/>
       <c r="C25" s="46" t="s">
-        <v>309</v>
+        <v>359</v>
       </c>
       <c r="D25" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>353</v>
+        <v>414</v>
       </c>
       <c r="F25" s="47"/>
     </row>
@@ -12630,45 +12654,45 @@
       <c r="A26" s="15"/>
       <c r="B26" s="72"/>
       <c r="C26" s="46" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F26" s="47"/>
     </row>
     <row r="27" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
-      <c r="B27" s="72"/>
+      <c r="A27" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="B27" s="72" t="s">
+        <v>125</v>
+      </c>
       <c r="C27" s="46" t="s">
-        <v>360</v>
+        <v>310</v>
       </c>
       <c r="D27" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>415</v>
+        <v>353</v>
       </c>
       <c r="F27" s="47"/>
     </row>
     <row r="28" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="B28" s="72" t="s">
-        <v>125</v>
-      </c>
+      <c r="A28" s="15"/>
+      <c r="B28" s="72"/>
       <c r="C28" s="46" t="s">
-        <v>310</v>
+        <v>361</v>
       </c>
       <c r="D28" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>353</v>
+        <v>414</v>
       </c>
       <c r="F28" s="47"/>
     </row>
@@ -12676,45 +12700,45 @@
       <c r="A29" s="15"/>
       <c r="B29" s="72"/>
       <c r="C29" s="46" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="D29" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F29" s="47"/>
     </row>
     <row r="30" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
-      <c r="B30" s="72"/>
+      <c r="A30" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="B30" s="72" t="s">
+        <v>126</v>
+      </c>
       <c r="C30" s="46" t="s">
-        <v>362</v>
+        <v>311</v>
       </c>
       <c r="D30" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>415</v>
+        <v>353</v>
       </c>
       <c r="F30" s="47"/>
     </row>
     <row r="31" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="B31" s="72" t="s">
-        <v>126</v>
-      </c>
+      <c r="A31" s="15"/>
+      <c r="B31" s="72"/>
       <c r="C31" s="46" t="s">
-        <v>311</v>
+        <v>363</v>
       </c>
       <c r="D31" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>353</v>
+        <v>414</v>
       </c>
       <c r="F31" s="47"/>
     </row>
@@ -12722,45 +12746,45 @@
       <c r="A32" s="15"/>
       <c r="B32" s="72"/>
       <c r="C32" s="46" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D32" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F32" s="47"/>
     </row>
     <row r="33" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="15"/>
-      <c r="B33" s="72"/>
+      <c r="A33" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="B33" s="72" t="s">
+        <v>127</v>
+      </c>
       <c r="C33" s="46" t="s">
-        <v>364</v>
+        <v>312</v>
       </c>
       <c r="D33" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>415</v>
+        <v>353</v>
       </c>
       <c r="F33" s="47"/>
     </row>
     <row r="34" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="B34" s="72" t="s">
-        <v>127</v>
-      </c>
+      <c r="A34" s="15"/>
+      <c r="B34" s="72"/>
       <c r="C34" s="46" t="s">
-        <v>312</v>
+        <v>365</v>
       </c>
       <c r="D34" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E34" s="18" t="s">
-        <v>353</v>
+        <v>414</v>
       </c>
       <c r="F34" s="47"/>
     </row>
@@ -12768,45 +12792,45 @@
       <c r="A35" s="15"/>
       <c r="B35" s="72"/>
       <c r="C35" s="46" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D35" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F35" s="47"/>
     </row>
     <row r="36" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="15"/>
-      <c r="B36" s="72"/>
+      <c r="A36" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="B36" s="72" t="s">
+        <v>128</v>
+      </c>
       <c r="C36" s="46" t="s">
-        <v>366</v>
+        <v>313</v>
       </c>
       <c r="D36" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>415</v>
+        <v>353</v>
       </c>
       <c r="F36" s="47"/>
     </row>
     <row r="37" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="B37" s="72" t="s">
-        <v>128</v>
-      </c>
+      <c r="A37" s="15"/>
+      <c r="B37" s="72"/>
       <c r="C37" s="46" t="s">
-        <v>313</v>
+        <v>367</v>
       </c>
       <c r="D37" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>353</v>
+        <v>414</v>
       </c>
       <c r="F37" s="47"/>
     </row>
@@ -12814,45 +12838,45 @@
       <c r="A38" s="15"/>
       <c r="B38" s="72"/>
       <c r="C38" s="46" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D38" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F38" s="47"/>
     </row>
     <row r="39" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
-      <c r="B39" s="72"/>
+      <c r="A39" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="B39" s="72" t="s">
+        <v>129</v>
+      </c>
       <c r="C39" s="46" t="s">
-        <v>368</v>
+        <v>314</v>
       </c>
       <c r="D39" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E39" s="18" t="s">
-        <v>415</v>
+        <v>353</v>
       </c>
       <c r="F39" s="47"/>
     </row>
     <row r="40" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="B40" s="72" t="s">
-        <v>129</v>
-      </c>
+      <c r="A40" s="15"/>
+      <c r="B40" s="72"/>
       <c r="C40" s="46" t="s">
-        <v>314</v>
+        <v>369</v>
       </c>
       <c r="D40" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>353</v>
+        <v>414</v>
       </c>
       <c r="F40" s="47"/>
     </row>
@@ -12860,45 +12884,45 @@
       <c r="A41" s="15"/>
       <c r="B41" s="72"/>
       <c r="C41" s="46" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="D41" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F41" s="47"/>
     </row>
     <row r="42" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="15"/>
-      <c r="B42" s="72"/>
+      <c r="A42" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="B42" s="72" t="s">
+        <v>130</v>
+      </c>
       <c r="C42" s="46" t="s">
-        <v>370</v>
+        <v>315</v>
       </c>
       <c r="D42" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E42" s="18" t="s">
-        <v>415</v>
+        <v>353</v>
       </c>
       <c r="F42" s="47"/>
     </row>
     <row r="43" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="B43" s="72" t="s">
-        <v>130</v>
-      </c>
+      <c r="A43" s="15"/>
+      <c r="B43" s="72"/>
       <c r="C43" s="46" t="s">
-        <v>315</v>
+        <v>371</v>
       </c>
       <c r="D43" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E43" s="18" t="s">
-        <v>353</v>
+        <v>414</v>
       </c>
       <c r="F43" s="47"/>
     </row>
@@ -12906,45 +12930,45 @@
       <c r="A44" s="15"/>
       <c r="B44" s="72"/>
       <c r="C44" s="46" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D44" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E44" s="18" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F44" s="47"/>
     </row>
     <row r="45" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="15"/>
-      <c r="B45" s="72"/>
-      <c r="C45" s="46" t="s">
-        <v>372</v>
+      <c r="A45" s="40" t="s">
+        <v>227</v>
+      </c>
+      <c r="B45" s="71" t="s">
+        <v>225</v>
+      </c>
+      <c r="C45" s="44" t="s">
+        <v>373</v>
       </c>
       <c r="D45" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E45" s="18" t="s">
-        <v>415</v>
+        <v>353</v>
       </c>
       <c r="F45" s="47"/>
     </row>
     <row r="46" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="40" t="s">
-        <v>227</v>
-      </c>
-      <c r="B46" s="71" t="s">
-        <v>225</v>
-      </c>
+      <c r="A46" s="40"/>
+      <c r="B46" s="71"/>
       <c r="C46" s="44" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D46" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E46" s="18" t="s">
-        <v>353</v>
+        <v>414</v>
       </c>
       <c r="F46" s="47"/>
     </row>
@@ -12952,45 +12976,45 @@
       <c r="A47" s="40"/>
       <c r="B47" s="71"/>
       <c r="C47" s="44" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D47" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E47" s="18" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F47" s="47"/>
     </row>
-    <row r="48" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="40"/>
-      <c r="B48" s="71"/>
+    <row r="48" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="40" t="s">
+        <v>228</v>
+      </c>
+      <c r="B48" s="71" t="s">
+        <v>226</v>
+      </c>
       <c r="C48" s="44" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="D48" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E48" s="18" t="s">
-        <v>415</v>
-      </c>
-      <c r="F48" s="47"/>
+        <v>353</v>
+      </c>
+      <c r="F48" s="44"/>
     </row>
     <row r="49" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="40" t="s">
-        <v>228</v>
-      </c>
-      <c r="B49" s="71" t="s">
-        <v>226</v>
-      </c>
+      <c r="A49" s="40"/>
+      <c r="B49" s="71"/>
       <c r="C49" s="44" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="D49" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E49" s="18" t="s">
-        <v>353</v>
+        <v>414</v>
       </c>
       <c r="F49" s="44"/>
     </row>
@@ -12998,45 +13022,45 @@
       <c r="A50" s="40"/>
       <c r="B50" s="71"/>
       <c r="C50" s="44" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="D50" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E50" s="18" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F50" s="44"/>
     </row>
     <row r="51" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="40"/>
-      <c r="B51" s="71"/>
-      <c r="C51" s="44" t="s">
-        <v>378</v>
+      <c r="A51" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="B51" s="72" t="s">
+        <v>146</v>
+      </c>
+      <c r="C51" s="46" t="s">
+        <v>379</v>
       </c>
       <c r="D51" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E51" s="18" t="s">
-        <v>415</v>
+        <v>353</v>
       </c>
       <c r="F51" s="44"/>
     </row>
     <row r="52" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="B52" s="72" t="s">
-        <v>146</v>
-      </c>
+      <c r="A52" s="15"/>
+      <c r="B52" s="72"/>
       <c r="C52" s="46" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D52" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E52" s="18" t="s">
-        <v>353</v>
+        <v>414</v>
       </c>
       <c r="F52" s="44"/>
     </row>
@@ -13044,91 +13068,91 @@
       <c r="A53" s="15"/>
       <c r="B53" s="72"/>
       <c r="C53" s="46" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="D53" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E53" s="18" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F53" s="44"/>
     </row>
     <row r="54" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="15"/>
-      <c r="B54" s="72"/>
-      <c r="C54" s="46" t="s">
-        <v>381</v>
+      <c r="A54" s="40" t="s">
+        <v>352</v>
+      </c>
+      <c r="B54" s="71"/>
+      <c r="C54" s="79" t="s">
+        <v>433</v>
       </c>
       <c r="D54" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E54" s="18" t="s">
-        <v>415</v>
-      </c>
-      <c r="F54" s="44"/>
+        <v>353</v>
+      </c>
+      <c r="F54" s="44" t="s">
+        <v>416</v>
+      </c>
     </row>
     <row r="55" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="40" t="s">
-        <v>352</v>
-      </c>
+      <c r="A55" s="40"/>
       <c r="B55" s="71"/>
-      <c r="C55" s="81" t="s">
-        <v>433</v>
+      <c r="C55" s="79" t="s">
+        <v>434</v>
       </c>
       <c r="D55" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E55" s="18" t="s">
-        <v>353</v>
-      </c>
-      <c r="F55" s="44" t="s">
-        <v>416</v>
-      </c>
+        <v>414</v>
+      </c>
+      <c r="F55" s="44"/>
     </row>
     <row r="56" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="40"/>
       <c r="B56" s="71"/>
-      <c r="C56" s="81" t="s">
-        <v>434</v>
+      <c r="C56" s="79" t="s">
+        <v>435</v>
       </c>
       <c r="D56" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E56" s="18" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F56" s="44"/>
     </row>
     <row r="57" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="40"/>
-      <c r="B57" s="71"/>
-      <c r="C57" s="81" t="s">
-        <v>435</v>
+      <c r="A57" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="B57" s="71" t="s">
+        <v>192</v>
+      </c>
+      <c r="C57" s="44" t="s">
+        <v>341</v>
       </c>
       <c r="D57" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E57" s="18" t="s">
-        <v>415</v>
+        <v>353</v>
       </c>
       <c r="F57" s="44"/>
     </row>
     <row r="58" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="B58" s="71" t="s">
-        <v>192</v>
-      </c>
+      <c r="A58" s="40"/>
+      <c r="B58" s="71"/>
       <c r="C58" s="44" t="s">
-        <v>341</v>
+        <v>382</v>
       </c>
       <c r="D58" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E58" s="18" t="s">
-        <v>353</v>
+        <v>414</v>
       </c>
       <c r="F58" s="44"/>
     </row>
@@ -13136,45 +13160,45 @@
       <c r="A59" s="40"/>
       <c r="B59" s="71"/>
       <c r="C59" s="44" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D59" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E59" s="18" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F59" s="44"/>
     </row>
     <row r="60" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="40"/>
-      <c r="B60" s="71"/>
+      <c r="A60" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="B60" s="71" t="s">
+        <v>193</v>
+      </c>
       <c r="C60" s="44" t="s">
-        <v>383</v>
+        <v>342</v>
       </c>
       <c r="D60" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E60" s="18" t="s">
-        <v>415</v>
+        <v>353</v>
       </c>
       <c r="F60" s="44"/>
     </row>
     <row r="61" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="40" t="s">
-        <v>190</v>
-      </c>
-      <c r="B61" s="71" t="s">
-        <v>193</v>
-      </c>
+      <c r="A61" s="40"/>
+      <c r="B61" s="71"/>
       <c r="C61" s="44" t="s">
-        <v>342</v>
+        <v>384</v>
       </c>
       <c r="D61" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E61" s="18" t="s">
-        <v>353</v>
+        <v>414</v>
       </c>
       <c r="F61" s="44"/>
     </row>
@@ -13182,45 +13206,45 @@
       <c r="A62" s="40"/>
       <c r="B62" s="71"/>
       <c r="C62" s="44" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D62" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E62" s="18" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F62" s="44"/>
     </row>
     <row r="63" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="40"/>
-      <c r="B63" s="71"/>
+      <c r="A63" s="40" t="s">
+        <v>191</v>
+      </c>
+      <c r="B63" s="71" t="s">
+        <v>194</v>
+      </c>
       <c r="C63" s="44" t="s">
-        <v>385</v>
+        <v>343</v>
       </c>
       <c r="D63" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E63" s="18" t="s">
-        <v>415</v>
+        <v>353</v>
       </c>
       <c r="F63" s="44"/>
     </row>
     <row r="64" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="40" t="s">
-        <v>191</v>
-      </c>
-      <c r="B64" s="71" t="s">
-        <v>194</v>
-      </c>
+      <c r="A64" s="40"/>
+      <c r="B64" s="71"/>
       <c r="C64" s="44" t="s">
-        <v>343</v>
+        <v>386</v>
       </c>
       <c r="D64" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E64" s="18" t="s">
-        <v>353</v>
+        <v>414</v>
       </c>
       <c r="F64" s="44"/>
     </row>
@@ -13228,45 +13252,45 @@
       <c r="A65" s="40"/>
       <c r="B65" s="71"/>
       <c r="C65" s="44" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="D65" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E65" s="18" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F65" s="44"/>
     </row>
     <row r="66" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="40"/>
-      <c r="B66" s="71"/>
+      <c r="A66" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="B66" s="71" t="s">
+        <v>223</v>
+      </c>
       <c r="C66" s="44" t="s">
-        <v>387</v>
+        <v>344</v>
       </c>
       <c r="D66" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E66" s="18" t="s">
-        <v>415</v>
+        <v>353</v>
       </c>
       <c r="F66" s="44"/>
     </row>
     <row r="67" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="40" t="s">
-        <v>189</v>
-      </c>
-      <c r="B67" s="71" t="s">
-        <v>223</v>
-      </c>
+      <c r="A67" s="40"/>
+      <c r="B67" s="71"/>
       <c r="C67" s="44" t="s">
-        <v>344</v>
+        <v>388</v>
       </c>
       <c r="D67" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E67" s="18" t="s">
-        <v>353</v>
+        <v>414</v>
       </c>
       <c r="F67" s="44"/>
     </row>
@@ -13274,37 +13298,41 @@
       <c r="A68" s="40"/>
       <c r="B68" s="71"/>
       <c r="C68" s="44" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="D68" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E68" s="18" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F68" s="44"/>
     </row>
-    <row r="69" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="40"/>
-      <c r="B69" s="71"/>
-      <c r="C69" s="44" t="s">
-        <v>389</v>
+    <row r="69" spans="1:6" s="42" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A69" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B69" s="72"/>
+      <c r="C69" s="80" t="s">
+        <v>438</v>
       </c>
       <c r="D69" s="18" t="s">
-        <v>413</v>
+        <v>419</v>
       </c>
       <c r="E69" s="18" t="s">
-        <v>415</v>
-      </c>
-      <c r="F69" s="44"/>
-    </row>
-    <row r="70" spans="1:6" s="42" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>424</v>
+      </c>
+      <c r="F69" s="47" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="15" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B70" s="72"/>
-      <c r="C70" s="82" t="s">
-        <v>438</v>
+      <c r="C70" s="46" t="s">
+        <v>390</v>
       </c>
       <c r="D70" s="18" t="s">
         <v>419</v>
@@ -13313,94 +13341,92 @@
         <v>424</v>
       </c>
       <c r="F70" s="47" t="s">
-        <v>423</v>
+        <v>101</v>
       </c>
     </row>
     <row r="71" spans="1:6" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="B71" s="72"/>
-      <c r="C71" s="46" t="s">
-        <v>390</v>
+      <c r="A71" s="40" t="s">
+        <v>275</v>
+      </c>
+      <c r="B71" s="71" t="s">
+        <v>288</v>
+      </c>
+      <c r="C71" s="44" t="s">
+        <v>440</v>
       </c>
       <c r="D71" s="18" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="E71" s="18" t="s">
-        <v>424</v>
+        <v>353</v>
       </c>
       <c r="F71" s="47" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A72" s="40" t="s">
-        <v>275</v>
-      </c>
-      <c r="B72" s="71" t="s">
-        <v>288</v>
-      </c>
+        <v>287</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="40"/>
+      <c r="B72" s="71"/>
       <c r="C72" s="44" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="D72" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E72" s="18" t="s">
-        <v>353</v>
+        <v>414</v>
       </c>
       <c r="F72" s="47" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="40"/>
       <c r="B73" s="71"/>
       <c r="C73" s="44" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="D73" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E73" s="18" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F73" s="47" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="74" spans="1:6" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="40"/>
-      <c r="B74" s="71"/>
+    <row r="74" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="40" t="s">
+        <v>276</v>
+      </c>
+      <c r="B74" s="71" t="s">
+        <v>289</v>
+      </c>
       <c r="C74" s="44" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="D74" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E74" s="18" t="s">
-        <v>415</v>
+        <v>353</v>
       </c>
       <c r="F74" s="47" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="75" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="40" t="s">
-        <v>276</v>
-      </c>
-      <c r="B75" s="71" t="s">
-        <v>289</v>
-      </c>
+      <c r="A75" s="40"/>
+      <c r="B75" s="71"/>
       <c r="C75" s="44" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="D75" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E75" s="18" t="s">
-        <v>353</v>
+        <v>414</v>
       </c>
       <c r="F75" s="47" t="s">
         <v>432</v>
@@ -13410,49 +13436,49 @@
       <c r="A76" s="40"/>
       <c r="B76" s="71"/>
       <c r="C76" s="44" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="D76" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E76" s="18" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F76" s="47" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="77" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="40"/>
-      <c r="B77" s="71"/>
+      <c r="A77" s="40" t="s">
+        <v>277</v>
+      </c>
+      <c r="B77" s="71" t="s">
+        <v>290</v>
+      </c>
       <c r="C77" s="44" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="D77" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E77" s="18" t="s">
-        <v>415</v>
+        <v>353</v>
       </c>
       <c r="F77" s="47" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="78" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="40" t="s">
-        <v>277</v>
-      </c>
-      <c r="B78" s="71" t="s">
-        <v>290</v>
-      </c>
+      <c r="A78" s="40"/>
+      <c r="B78" s="71"/>
       <c r="C78" s="44" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="D78" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E78" s="18" t="s">
-        <v>353</v>
+        <v>414</v>
       </c>
       <c r="F78" s="47" t="s">
         <v>432</v>
@@ -13462,41 +13488,43 @@
       <c r="A79" s="40"/>
       <c r="B79" s="71"/>
       <c r="C79" s="44" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="D79" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E79" s="18" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F79" s="47" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="80" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="40"/>
-      <c r="B80" s="71"/>
-      <c r="C80" s="44" t="s">
-        <v>448</v>
+    <row r="80" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A80" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B80" s="72"/>
+      <c r="C80" s="80" t="s">
+        <v>439</v>
       </c>
       <c r="D80" s="18" t="s">
-        <v>413</v>
+        <v>419</v>
       </c>
       <c r="E80" s="18" t="s">
-        <v>415</v>
+        <v>424</v>
       </c>
       <c r="F80" s="47" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="15" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B81" s="72"/>
-      <c r="C81" s="82" t="s">
-        <v>439</v>
+      <c r="C81" s="46" t="s">
+        <v>391</v>
       </c>
       <c r="D81" s="18" t="s">
         <v>419</v>
@@ -13505,46 +13533,44 @@
         <v>424</v>
       </c>
       <c r="F81" s="47" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" s="42" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A82" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B82" s="72"/>
+        <v>102</v>
+      </c>
+      <c r="B82" s="72" t="s">
+        <v>291</v>
+      </c>
       <c r="C82" s="46" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D82" s="18" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="E82" s="18" t="s">
-        <v>424</v>
+        <v>353</v>
       </c>
       <c r="F82" s="47" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" s="42" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A83" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="B83" s="72" t="s">
-        <v>291</v>
-      </c>
+        <v>278</v>
+      </c>
+      <c r="G82" s="12"/>
+      <c r="H82" s="12"/>
+    </row>
+    <row r="83" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="15"/>
+      <c r="B83" s="72"/>
       <c r="C83" s="46" t="s">
-        <v>392</v>
+        <v>449</v>
       </c>
       <c r="D83" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E83" s="18" t="s">
-        <v>353</v>
-      </c>
-      <c r="F83" s="47" t="s">
-        <v>278</v>
-      </c>
+        <v>414</v>
+      </c>
+      <c r="F83" s="47"/>
       <c r="G83" s="12"/>
       <c r="H83" s="12"/>
     </row>
@@ -13552,53 +13578,53 @@
       <c r="A84" s="15"/>
       <c r="B84" s="72"/>
       <c r="C84" s="46" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="D84" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E84" s="18" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F84" s="47"/>
       <c r="G84" s="12"/>
       <c r="H84" s="12"/>
     </row>
-    <row r="85" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="15"/>
-      <c r="B85" s="72"/>
+    <row r="85" spans="1:8" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A85" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="B85" s="72" t="s">
+        <v>280</v>
+      </c>
       <c r="C85" s="46" t="s">
-        <v>450</v>
+        <v>393</v>
       </c>
       <c r="D85" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E85" s="18" t="s">
-        <v>415</v>
-      </c>
-      <c r="F85" s="47"/>
+        <v>353</v>
+      </c>
+      <c r="F85" s="15" t="s">
+        <v>429</v>
+      </c>
       <c r="G85" s="12"/>
       <c r="H85" s="12"/>
     </row>
-    <row r="86" spans="1:8" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A86" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="B86" s="72" t="s">
-        <v>280</v>
-      </c>
+    <row r="86" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="15"/>
+      <c r="B86" s="72"/>
       <c r="C86" s="46" t="s">
-        <v>393</v>
+        <v>451</v>
       </c>
       <c r="D86" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E86" s="18" t="s">
-        <v>353</v>
-      </c>
-      <c r="F86" s="15" t="s">
-        <v>429</v>
-      </c>
+        <v>414</v>
+      </c>
+      <c r="F86" s="12"/>
       <c r="G86" s="12"/>
       <c r="H86" s="12"/>
     </row>
@@ -13606,53 +13632,53 @@
       <c r="A87" s="15"/>
       <c r="B87" s="72"/>
       <c r="C87" s="46" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="D87" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E87" s="18" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F87" s="12"/>
       <c r="G87" s="12"/>
       <c r="H87" s="12"/>
     </row>
     <row r="88" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="15"/>
-      <c r="B88" s="72"/>
+      <c r="A88" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="B88" s="72" t="s">
+        <v>124</v>
+      </c>
       <c r="C88" s="46" t="s">
-        <v>452</v>
+        <v>394</v>
       </c>
       <c r="D88" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E88" s="18" t="s">
-        <v>415</v>
-      </c>
-      <c r="F88" s="12"/>
+        <v>353</v>
+      </c>
+      <c r="F88" s="12" t="s">
+        <v>279</v>
+      </c>
       <c r="G88" s="12"/>
       <c r="H88" s="12"/>
     </row>
     <row r="89" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="B89" s="72" t="s">
-        <v>124</v>
-      </c>
+      <c r="A89" s="15"/>
+      <c r="B89" s="72"/>
       <c r="C89" s="46" t="s">
-        <v>394</v>
+        <v>453</v>
       </c>
       <c r="D89" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E89" s="18" t="s">
-        <v>353</v>
-      </c>
-      <c r="F89" s="12" t="s">
-        <v>279</v>
-      </c>
+        <v>414</v>
+      </c>
+      <c r="F89" s="12"/>
       <c r="G89" s="12"/>
       <c r="H89" s="12"/>
     </row>
@@ -13660,107 +13686,107 @@
       <c r="A90" s="15"/>
       <c r="B90" s="72"/>
       <c r="C90" s="46" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="D90" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E90" s="18" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F90" s="12"/>
       <c r="G90" s="12"/>
       <c r="H90" s="12"/>
     </row>
-    <row r="91" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="15"/>
-      <c r="B91" s="72"/>
-      <c r="C91" s="46" t="s">
-        <v>454</v>
+    <row r="91" spans="1:8" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A91" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B91" s="72" t="s">
+        <v>281</v>
+      </c>
+      <c r="C91" s="81" t="s">
+        <v>395</v>
       </c>
       <c r="D91" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E91" s="18" t="s">
-        <v>415</v>
-      </c>
-      <c r="F91" s="12"/>
+        <v>353</v>
+      </c>
+      <c r="F91" s="15" t="s">
+        <v>429</v>
+      </c>
       <c r="G91" s="12"/>
       <c r="H91" s="12"/>
     </row>
-    <row r="92" spans="1:8" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A92" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="B92" s="72" t="s">
-        <v>281</v>
-      </c>
-      <c r="C92" s="83" t="s">
-        <v>395</v>
+    <row r="92" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="15"/>
+      <c r="B92" s="72"/>
+      <c r="C92" s="81" t="s">
+        <v>455</v>
       </c>
       <c r="D92" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E92" s="18" t="s">
-        <v>353</v>
-      </c>
-      <c r="F92" s="15" t="s">
-        <v>429</v>
-      </c>
+        <v>414</v>
+      </c>
+      <c r="F92" s="12"/>
       <c r="G92" s="12"/>
       <c r="H92" s="12"/>
     </row>
     <row r="93" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="15"/>
       <c r="B93" s="72"/>
-      <c r="C93" s="83" t="s">
-        <v>455</v>
+      <c r="C93" s="81" t="s">
+        <v>456</v>
       </c>
       <c r="D93" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E93" s="18" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F93" s="12"/>
       <c r="G93" s="12"/>
       <c r="H93" s="12"/>
     </row>
     <row r="94" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="15"/>
-      <c r="B94" s="72"/>
-      <c r="C94" s="83" t="s">
-        <v>456</v>
+      <c r="A94" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B94" s="72" t="s">
+        <v>130</v>
+      </c>
+      <c r="C94" s="46" t="s">
+        <v>396</v>
       </c>
       <c r="D94" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E94" s="18" t="s">
-        <v>415</v>
-      </c>
-      <c r="F94" s="12"/>
+        <v>353</v>
+      </c>
+      <c r="F94" s="12" t="s">
+        <v>279</v>
+      </c>
       <c r="G94" s="12"/>
       <c r="H94" s="12"/>
     </row>
     <row r="95" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="B95" s="72" t="s">
-        <v>130</v>
-      </c>
+      <c r="A95" s="15"/>
+      <c r="B95" s="72"/>
       <c r="C95" s="46" t="s">
-        <v>396</v>
+        <v>457</v>
       </c>
       <c r="D95" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E95" s="18" t="s">
-        <v>353</v>
-      </c>
-      <c r="F95" s="12" t="s">
-        <v>279</v>
-      </c>
+        <v>414</v>
+      </c>
+      <c r="F95" s="12"/>
       <c r="G95" s="12"/>
       <c r="H95" s="12"/>
     </row>
@@ -13768,53 +13794,53 @@
       <c r="A96" s="15"/>
       <c r="B96" s="72"/>
       <c r="C96" s="46" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="D96" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E96" s="18" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F96" s="12"/>
       <c r="G96" s="12"/>
       <c r="H96" s="12"/>
     </row>
-    <row r="97" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="15"/>
-      <c r="B97" s="72"/>
+    <row r="97" spans="1:8" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A97" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B97" s="72" t="s">
+        <v>282</v>
+      </c>
       <c r="C97" s="46" t="s">
-        <v>458</v>
+        <v>397</v>
       </c>
       <c r="D97" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E97" s="18" t="s">
-        <v>415</v>
-      </c>
-      <c r="F97" s="12"/>
+        <v>353</v>
+      </c>
+      <c r="F97" s="15" t="s">
+        <v>429</v>
+      </c>
       <c r="G97" s="12"/>
       <c r="H97" s="12"/>
     </row>
-    <row r="98" spans="1:8" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="B98" s="72" t="s">
-        <v>282</v>
-      </c>
+    <row r="98" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="15"/>
+      <c r="B98" s="72"/>
       <c r="C98" s="46" t="s">
-        <v>397</v>
+        <v>459</v>
       </c>
       <c r="D98" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E98" s="18" t="s">
-        <v>353</v>
-      </c>
-      <c r="F98" s="15" t="s">
-        <v>429</v>
-      </c>
+        <v>414</v>
+      </c>
+      <c r="F98" s="12"/>
       <c r="G98" s="12"/>
       <c r="H98" s="12"/>
     </row>
@@ -13822,53 +13848,53 @@
       <c r="A99" s="15"/>
       <c r="B99" s="72"/>
       <c r="C99" s="46" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="D99" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E99" s="18" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F99" s="12"/>
       <c r="G99" s="12"/>
       <c r="H99" s="12"/>
     </row>
     <row r="100" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="15"/>
-      <c r="B100" s="72"/>
+      <c r="A100" s="15" t="s">
+        <v>283</v>
+      </c>
+      <c r="B100" s="72" t="s">
+        <v>290</v>
+      </c>
       <c r="C100" s="46" t="s">
-        <v>460</v>
+        <v>398</v>
       </c>
       <c r="D100" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E100" s="18" t="s">
-        <v>415</v>
-      </c>
-      <c r="F100" s="12"/>
+        <v>353</v>
+      </c>
+      <c r="F100" s="12" t="s">
+        <v>279</v>
+      </c>
       <c r="G100" s="12"/>
       <c r="H100" s="12"/>
     </row>
     <row r="101" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="15" t="s">
-        <v>283</v>
-      </c>
-      <c r="B101" s="72" t="s">
-        <v>290</v>
-      </c>
+      <c r="A101" s="15"/>
+      <c r="B101" s="72"/>
       <c r="C101" s="46" t="s">
-        <v>398</v>
+        <v>461</v>
       </c>
       <c r="D101" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E101" s="18" t="s">
-        <v>353</v>
-      </c>
-      <c r="F101" s="12" t="s">
-        <v>279</v>
-      </c>
+        <v>414</v>
+      </c>
+      <c r="F101" s="12"/>
       <c r="G101" s="12"/>
       <c r="H101" s="12"/>
     </row>
@@ -13876,101 +13902,113 @@
       <c r="A102" s="15"/>
       <c r="B102" s="72"/>
       <c r="C102" s="46" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="D102" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E102" s="18" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F102" s="12"/>
       <c r="G102" s="12"/>
       <c r="H102" s="12"/>
     </row>
-    <row r="103" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="15"/>
-      <c r="B103" s="72"/>
+    <row r="103" spans="1:8" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A103" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="B103" s="72" t="s">
+        <v>285</v>
+      </c>
       <c r="C103" s="46" t="s">
-        <v>462</v>
+        <v>399</v>
       </c>
       <c r="D103" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E103" s="18" t="s">
-        <v>415</v>
-      </c>
-      <c r="F103" s="12"/>
+        <v>353</v>
+      </c>
+      <c r="F103" s="15" t="s">
+        <v>429</v>
+      </c>
       <c r="G103" s="12"/>
       <c r="H103" s="12"/>
     </row>
-    <row r="104" spans="1:8" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A104" s="15" t="s">
-        <v>284</v>
-      </c>
-      <c r="B104" s="72" t="s">
-        <v>285</v>
-      </c>
+    <row r="104" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="15"/>
+      <c r="B104" s="72"/>
       <c r="C104" s="46" t="s">
-        <v>399</v>
+        <v>463</v>
       </c>
       <c r="D104" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E104" s="18" t="s">
-        <v>353</v>
-      </c>
-      <c r="F104" s="15" t="s">
-        <v>429</v>
-      </c>
+        <v>414</v>
+      </c>
+      <c r="F104" s="47"/>
       <c r="G104" s="12"/>
       <c r="H104" s="12"/>
     </row>
     <row r="105" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="15"/>
-      <c r="B105" s="72"/>
-      <c r="C105" s="46" t="s">
-        <v>463</v>
+      <c r="A105" s="40"/>
+      <c r="B105" s="71"/>
+      <c r="C105" s="44" t="s">
+        <v>464</v>
       </c>
       <c r="D105" s="18" t="s">
         <v>413</v>
       </c>
       <c r="E105" s="18" t="s">
-        <v>414</v>
-      </c>
-      <c r="F105" s="47"/>
-      <c r="G105" s="12"/>
-      <c r="H105" s="12"/>
+        <v>415</v>
+      </c>
+      <c r="F105" s="44"/>
     </row>
     <row r="106" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="40"/>
-      <c r="B106" s="71"/>
-      <c r="C106" s="44" t="s">
-        <v>464</v>
-      </c>
-      <c r="D106" s="18" t="s">
-        <v>413</v>
-      </c>
-      <c r="E106" s="18" t="s">
-        <v>415</v>
-      </c>
-      <c r="F106" s="44"/>
+      <c r="A106" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="B106" s="72"/>
+      <c r="C106" s="45" t="s">
+        <v>465</v>
+      </c>
+      <c r="D106" s="41" t="s">
+        <v>419</v>
+      </c>
+      <c r="E106" s="41" t="s">
+        <v>425</v>
+      </c>
+      <c r="F106" s="44" t="s">
+        <v>426</v>
+      </c>
     </row>
     <row r="107" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="40"/>
-      <c r="B107" s="71"/>
-      <c r="C107" s="44"/>
-      <c r="D107" s="18"/>
-      <c r="E107" s="18"/>
-      <c r="F107" s="44"/>
+      <c r="A107" s="40" t="s">
+        <v>95</v>
+      </c>
+      <c r="B107" s="72"/>
+      <c r="C107" s="45" t="s">
+        <v>467</v>
+      </c>
+      <c r="D107" s="41" t="s">
+        <v>419</v>
+      </c>
+      <c r="E107" s="41" t="s">
+        <v>425</v>
+      </c>
+      <c r="F107" s="44" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="108" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="40" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B108" s="72"/>
       <c r="C108" s="45" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="D108" s="41" t="s">
         <v>419</v>
@@ -13978,17 +14016,15 @@
       <c r="E108" s="41" t="s">
         <v>425</v>
       </c>
-      <c r="F108" s="44" t="s">
-        <v>426</v>
-      </c>
+      <c r="F108" s="44"/>
     </row>
     <row r="109" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="40" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B109" s="72"/>
       <c r="C109" s="45" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="D109" s="41" t="s">
         <v>419</v>
@@ -13996,86 +14032,107 @@
       <c r="E109" s="41" t="s">
         <v>425</v>
       </c>
-      <c r="F109" s="44" t="s">
-        <v>420</v>
-      </c>
+      <c r="F109" s="44"/>
     </row>
     <row r="110" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="40" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B110" s="72"/>
       <c r="C110" s="45" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
       <c r="D110" s="41" t="s">
         <v>419</v>
       </c>
       <c r="E110" s="41" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="F110" s="44"/>
     </row>
-    <row r="111" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="40" t="s">
-        <v>96</v>
+    <row r="111" spans="1:8" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>98</v>
       </c>
       <c r="B111" s="72"/>
-      <c r="C111" s="45" t="s">
-        <v>468</v>
-      </c>
-      <c r="D111" s="41" t="s">
-        <v>419</v>
-      </c>
-      <c r="E111" s="41" t="s">
-        <v>425</v>
-      </c>
-      <c r="F111" s="44"/>
-    </row>
-    <row r="112" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="40" t="s">
-        <v>97</v>
-      </c>
-      <c r="B112" s="72"/>
-      <c r="C112" s="45" t="s">
-        <v>469</v>
+      <c r="C111" s="78" t="s">
+        <v>470</v>
+      </c>
+      <c r="D111" s="18" t="s">
+        <v>418</v>
+      </c>
+      <c r="E111" s="18" t="s">
+        <v>418</v>
+      </c>
+      <c r="F111" s="47" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A112" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B112" s="73" t="s">
+        <v>99</v>
+      </c>
+      <c r="C112" t="s">
+        <v>345</v>
       </c>
       <c r="D112" s="41" t="s">
         <v>419</v>
       </c>
       <c r="E112" s="41" t="s">
+        <v>347</v>
+      </c>
+      <c r="F112" s="47" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A113" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B113" s="73" t="s">
+        <v>100</v>
+      </c>
+      <c r="C113" t="s">
+        <v>346</v>
+      </c>
+      <c r="D113" s="41" t="s">
         <v>419</v>
       </c>
-      <c r="F112" s="44"/>
-    </row>
-    <row r="113" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="E113" s="41" t="s">
+        <v>347</v>
+      </c>
+      <c r="F113" s="47" t="s">
+        <v>428</v>
+      </c>
+    </row>
     <row r="114" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>98</v>
-      </c>
-      <c r="B114" s="72"/>
-      <c r="C114" s="80" t="s">
-        <v>470</v>
-      </c>
-      <c r="D114" s="18" t="s">
-        <v>418</v>
-      </c>
-      <c r="E114" s="18" t="s">
-        <v>418</v>
+      <c r="A114" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B114" s="73"/>
+      <c r="C114" t="s">
+        <v>471</v>
+      </c>
+      <c r="D114" s="41" t="s">
+        <v>419</v>
+      </c>
+      <c r="E114" s="41" t="s">
+        <v>347</v>
       </c>
       <c r="F114" s="47" t="s">
-        <v>348</v>
+        <v>430</v>
       </c>
     </row>
     <row r="115" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="B115" s="73" t="s">
-        <v>99</v>
-      </c>
-      <c r="C115" t="s">
-        <v>345</v>
+        <v>84</v>
+      </c>
+      <c r="B115" s="72"/>
+      <c r="C115" s="46" t="s">
+        <v>472</v>
       </c>
       <c r="D115" s="41" t="s">
         <v>419</v>
@@ -14084,122 +14141,134 @@
         <v>347</v>
       </c>
       <c r="F115" s="47" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
     </row>
     <row r="116" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="B116" s="73" t="s">
-        <v>100</v>
-      </c>
-      <c r="C116" t="s">
-        <v>346</v>
-      </c>
-      <c r="D116" s="41" t="s">
-        <v>419</v>
-      </c>
-      <c r="E116" s="41" t="s">
-        <v>347</v>
+        <v>32</v>
+      </c>
+      <c r="B116" s="72"/>
+      <c r="C116" s="46" t="s">
+        <v>473</v>
+      </c>
+      <c r="D116" s="18" t="s">
+        <v>418</v>
+      </c>
+      <c r="E116" s="18" t="s">
+        <v>418</v>
       </c>
       <c r="F116" s="47" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="B117" s="73"/>
-      <c r="C117" t="s">
-        <v>471</v>
-      </c>
-      <c r="D117" s="41" t="s">
-        <v>419</v>
-      </c>
-      <c r="E117" s="41" t="s">
-        <v>347</v>
-      </c>
-      <c r="F117" s="47" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>400</v>
+      </c>
+      <c r="B117" s="72"/>
+      <c r="C117" s="46" t="s">
+        <v>401</v>
+      </c>
+      <c r="D117" s="18" t="s">
+        <v>418</v>
+      </c>
+      <c r="E117" s="18" t="s">
+        <v>418</v>
+      </c>
+      <c r="F117" s="47"/>
+    </row>
+    <row r="118" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A118" s="15" t="s">
-        <v>84</v>
+        <v>319</v>
       </c>
       <c r="B118" s="72"/>
       <c r="C118" s="46" t="s">
-        <v>472</v>
-      </c>
-      <c r="D118" s="41" t="s">
-        <v>419</v>
-      </c>
-      <c r="E118" s="41" t="s">
-        <v>347</v>
+        <v>318</v>
+      </c>
+      <c r="D118" s="18" t="s">
+        <v>413</v>
+      </c>
+      <c r="E118" s="18" t="s">
+        <v>353</v>
       </c>
       <c r="F118" s="47" t="s">
-        <v>430</v>
+        <v>316</v>
       </c>
     </row>
     <row r="119" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="15"/>
+      <c r="A119" s="15" t="s">
+        <v>320</v>
+      </c>
       <c r="B119" s="72"/>
-      <c r="C119" s="46"/>
-      <c r="D119" s="18"/>
-      <c r="E119" s="18"/>
+      <c r="C119" s="46" t="s">
+        <v>322</v>
+      </c>
+      <c r="D119" s="18" t="s">
+        <v>413</v>
+      </c>
+      <c r="E119" s="18" t="s">
+        <v>353</v>
+      </c>
       <c r="F119" s="47"/>
     </row>
     <row r="120" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A120" s="15" t="s">
-        <v>32</v>
+        <v>321</v>
       </c>
       <c r="B120" s="72"/>
       <c r="C120" s="46" t="s">
-        <v>473</v>
+        <v>323</v>
       </c>
       <c r="D120" s="18" t="s">
+        <v>413</v>
+      </c>
+      <c r="E120" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="F120" s="47"/>
+    </row>
+    <row r="121" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="15" t="s">
+        <v>402</v>
+      </c>
+      <c r="B121" s="72"/>
+      <c r="C121" s="46" t="s">
+        <v>403</v>
+      </c>
+      <c r="D121" s="18" t="s">
         <v>418</v>
       </c>
-      <c r="E120" s="18" t="s">
+      <c r="E121" s="18" t="s">
         <v>418</v>
       </c>
-      <c r="F120" s="47" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="15"/>
-      <c r="B121" s="72"/>
-      <c r="C121" s="46"/>
-      <c r="D121" s="18"/>
-      <c r="E121" s="18"/>
       <c r="F121" s="47"/>
     </row>
     <row r="122" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="15" t="s">
-        <v>400</v>
+        <v>325</v>
       </c>
       <c r="B122" s="72"/>
       <c r="C122" s="46" t="s">
-        <v>401</v>
+        <v>340</v>
       </c>
       <c r="D122" s="18" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="E122" s="18" t="s">
-        <v>418</v>
-      </c>
-      <c r="F122" s="47"/>
-    </row>
-    <row r="123" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+      <c r="F122" s="47" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="15" t="s">
-        <v>319</v>
+        <v>326</v>
       </c>
       <c r="B123" s="72"/>
       <c r="C123" s="46" t="s">
-        <v>318</v>
+        <v>339</v>
       </c>
       <c r="D123" s="18" t="s">
         <v>413</v>
@@ -14207,17 +14276,14 @@
       <c r="E123" s="18" t="s">
         <v>353</v>
       </c>
-      <c r="F123" s="47" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="124" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A124" s="15" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
       <c r="B124" s="72"/>
       <c r="C124" s="46" t="s">
-        <v>322</v>
+        <v>338</v>
       </c>
       <c r="D124" s="18" t="s">
         <v>413</v>
@@ -14225,31 +14291,33 @@
       <c r="E124" s="18" t="s">
         <v>353</v>
       </c>
-      <c r="F124" s="47"/>
-    </row>
-    <row r="125" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F124" s="15" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="15" t="s">
-        <v>321</v>
+        <v>404</v>
       </c>
       <c r="B125" s="72"/>
       <c r="C125" s="46" t="s">
-        <v>323</v>
+        <v>405</v>
       </c>
       <c r="D125" s="18" t="s">
-        <v>413</v>
+        <v>418</v>
       </c>
       <c r="E125" s="18" t="s">
-        <v>353</v>
+        <v>418</v>
       </c>
       <c r="F125" s="47"/>
     </row>
     <row r="126" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="15" t="s">
-        <v>317</v>
+        <v>329</v>
       </c>
       <c r="B126" s="72"/>
       <c r="C126" s="46" t="s">
-        <v>324</v>
+        <v>336</v>
       </c>
       <c r="D126" s="18" t="s">
         <v>413</v>
@@ -14261,27 +14329,27 @@
     </row>
     <row r="127" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="15" t="s">
-        <v>402</v>
+        <v>330</v>
       </c>
       <c r="B127" s="72"/>
       <c r="C127" s="46" t="s">
-        <v>403</v>
+        <v>335</v>
       </c>
       <c r="D127" s="18" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="E127" s="18" t="s">
-        <v>418</v>
+        <v>353</v>
       </c>
       <c r="F127" s="47"/>
     </row>
-    <row r="128" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A128" s="15" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="B128" s="72"/>
       <c r="C128" s="46" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="D128" s="18" t="s">
         <v>413</v>
@@ -14289,173 +14357,115 @@
       <c r="E128" s="18" t="s">
         <v>353</v>
       </c>
-      <c r="F128" s="47" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="15" t="s">
-        <v>326</v>
-      </c>
-      <c r="B129" s="72"/>
-      <c r="C129" s="46" t="s">
-        <v>339</v>
-      </c>
-      <c r="D129" s="18" t="s">
-        <v>413</v>
-      </c>
-      <c r="E129" s="18" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A130" s="15" t="s">
-        <v>327</v>
-      </c>
+      <c r="F128" s="47"/>
+    </row>
+    <row r="130" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="15"/>
       <c r="B130" s="72"/>
-      <c r="C130" s="46" t="s">
-        <v>338</v>
-      </c>
-      <c r="D130" s="18" t="s">
-        <v>413</v>
-      </c>
-      <c r="E130" s="18" t="s">
-        <v>353</v>
-      </c>
-      <c r="F130" s="15" t="s">
-        <v>406</v>
-      </c>
+      <c r="C130" s="46"/>
+      <c r="D130" s="18"/>
+      <c r="E130" s="18"/>
+      <c r="F130" s="47"/>
     </row>
     <row r="131" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="15" t="s">
-        <v>328</v>
-      </c>
       <c r="B131" s="72"/>
-      <c r="C131" s="46" t="s">
-        <v>337</v>
-      </c>
-      <c r="D131" s="18" t="s">
-        <v>413</v>
-      </c>
-      <c r="E131" s="18" t="s">
-        <v>353</v>
-      </c>
+      <c r="C131" s="46"/>
+      <c r="D131" s="18"/>
+      <c r="E131" s="18"/>
       <c r="F131" s="47"/>
     </row>
     <row r="132" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="15" t="s">
-        <v>404</v>
-      </c>
-      <c r="B132" s="72"/>
-      <c r="C132" s="46" t="s">
-        <v>405</v>
-      </c>
-      <c r="D132" s="18" t="s">
-        <v>418</v>
-      </c>
-      <c r="E132" s="18" t="s">
-        <v>418</v>
-      </c>
+      <c r="A132" s="15"/>
+      <c r="B132" s="46"/>
+      <c r="C132" s="46"/>
+      <c r="D132" s="18"/>
+      <c r="E132" s="18"/>
       <c r="F132" s="47"/>
     </row>
     <row r="133" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="15" t="s">
-        <v>329</v>
-      </c>
-      <c r="B133" s="72"/>
-      <c r="C133" s="46" t="s">
-        <v>336</v>
-      </c>
-      <c r="D133" s="18" t="s">
-        <v>413</v>
-      </c>
-      <c r="E133" s="18" t="s">
-        <v>353</v>
-      </c>
+      <c r="A133" s="15"/>
+      <c r="B133" s="46"/>
+      <c r="C133" s="46"/>
+      <c r="D133" s="18"/>
+      <c r="E133" s="18"/>
       <c r="F133" s="47"/>
     </row>
     <row r="134" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="15" t="s">
-        <v>330</v>
-      </c>
-      <c r="B134" s="72"/>
-      <c r="C134" s="46" t="s">
-        <v>335</v>
-      </c>
-      <c r="D134" s="18" t="s">
-        <v>413</v>
-      </c>
-      <c r="E134" s="18" t="s">
-        <v>353</v>
-      </c>
+      <c r="A134" s="15"/>
+      <c r="B134" s="46"/>
+      <c r="C134" s="46"/>
+      <c r="D134" s="18"/>
+      <c r="E134" s="18"/>
       <c r="F134" s="47"/>
     </row>
-    <row r="135" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A135" s="15" t="s">
-        <v>331</v>
-      </c>
-      <c r="B135" s="72"/>
-      <c r="C135" s="46" t="s">
-        <v>334</v>
-      </c>
-      <c r="D135" s="18" t="s">
-        <v>413</v>
-      </c>
-      <c r="E135" s="18" t="s">
-        <v>353</v>
-      </c>
+    <row r="135" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="15"/>
+      <c r="B135" s="46"/>
+      <c r="C135" s="46"/>
+      <c r="D135" s="18"/>
+      <c r="E135" s="18"/>
       <c r="F135" s="47"/>
     </row>
     <row r="136" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="15" t="s">
-        <v>332</v>
-      </c>
-      <c r="B136" s="72"/>
-      <c r="C136" s="46" t="s">
-        <v>333</v>
-      </c>
-      <c r="D136" s="18" t="s">
-        <v>413</v>
-      </c>
-      <c r="E136" s="18" t="s">
-        <v>353</v>
-      </c>
+      <c r="A136" s="15"/>
+      <c r="B136" s="46"/>
+      <c r="C136" s="46"/>
+      <c r="D136" s="18"/>
+      <c r="E136" s="18"/>
       <c r="F136" s="47"/>
     </row>
     <row r="137" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="15"/>
-      <c r="B137" s="72"/>
+      <c r="B137" s="46"/>
       <c r="C137" s="46"/>
       <c r="D137" s="18"/>
       <c r="E137" s="18"/>
       <c r="F137" s="47"/>
     </row>
     <row r="138" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B138" s="72"/>
+      <c r="A138" s="76" t="s">
+        <v>407</v>
+      </c>
+      <c r="B138" s="77">
+        <f>(B139*B140*1440*B141) / 10000000</f>
+        <v>3.024</v>
+      </c>
       <c r="C138" s="46"/>
       <c r="D138" s="18"/>
       <c r="E138" s="18"/>
       <c r="F138" s="47"/>
     </row>
     <row r="139" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="15"/>
-      <c r="B139" s="46"/>
+      <c r="A139" s="74" t="s">
+        <v>408</v>
+      </c>
+      <c r="B139" s="75">
+        <v>150</v>
+      </c>
       <c r="C139" s="46"/>
       <c r="D139" s="18"/>
       <c r="E139" s="18"/>
       <c r="F139" s="47"/>
     </row>
     <row r="140" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="15"/>
-      <c r="B140" s="46"/>
+      <c r="A140" s="74" t="s">
+        <v>409</v>
+      </c>
+      <c r="B140" s="75">
+        <v>7</v>
+      </c>
       <c r="C140" s="46"/>
       <c r="D140" s="18"/>
       <c r="E140" s="18"/>
       <c r="F140" s="47"/>
     </row>
     <row r="141" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="15"/>
-      <c r="B141" s="46"/>
+      <c r="A141" s="74" t="s">
+        <v>410</v>
+      </c>
+      <c r="B141" s="75">
+        <v>20</v>
+      </c>
       <c r="C141" s="46"/>
       <c r="D141" s="18"/>
       <c r="E141" s="18"/>
@@ -14486,49 +14496,32 @@
       <c r="F144" s="47"/>
     </row>
     <row r="145" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="76" t="s">
-        <v>407</v>
-      </c>
-      <c r="B145" s="77">
-        <f>(B146*B147*1440*B148) / 10000000</f>
-        <v>3.024</v>
-      </c>
+      <c r="A145" s="15"/>
+      <c r="B145" s="46"/>
       <c r="C145" s="46"/>
       <c r="D145" s="18"/>
       <c r="E145" s="18"/>
       <c r="F145" s="47"/>
     </row>
     <row r="146" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="74" t="s">
-        <v>408</v>
-      </c>
-      <c r="B146" s="75">
-        <v>150</v>
-      </c>
+      <c r="A146" s="15"/>
+      <c r="B146" s="46"/>
       <c r="C146" s="46"/>
       <c r="D146" s="18"/>
       <c r="E146" s="18"/>
       <c r="F146" s="47"/>
     </row>
     <row r="147" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="74" t="s">
-        <v>409</v>
-      </c>
-      <c r="B147" s="75">
-        <v>7</v>
-      </c>
+      <c r="A147" s="15"/>
+      <c r="B147" s="46"/>
       <c r="C147" s="46"/>
       <c r="D147" s="18"/>
       <c r="E147" s="18"/>
       <c r="F147" s="47"/>
     </row>
     <row r="148" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="74" t="s">
-        <v>410</v>
-      </c>
-      <c r="B148" s="75">
-        <v>20</v>
-      </c>
+      <c r="A148" s="15"/>
+      <c r="B148" s="46"/>
       <c r="C148" s="46"/>
       <c r="D148" s="18"/>
       <c r="E148" s="18"/>
@@ -14544,56 +14537,42 @@
     </row>
     <row r="150" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A150" s="15"/>
-      <c r="B150" s="46"/>
-      <c r="C150" s="46"/>
       <c r="D150" s="18"/>
       <c r="E150" s="18"/>
       <c r="F150" s="47"/>
     </row>
     <row r="151" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A151" s="15"/>
-      <c r="B151" s="46"/>
-      <c r="C151" s="46"/>
       <c r="D151" s="18"/>
       <c r="E151" s="18"/>
       <c r="F151" s="47"/>
     </row>
     <row r="152" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A152" s="15"/>
-      <c r="B152" s="46"/>
-      <c r="C152" s="46"/>
       <c r="D152" s="18"/>
       <c r="E152" s="18"/>
       <c r="F152" s="47"/>
     </row>
     <row r="153" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A153" s="15"/>
-      <c r="B153" s="46"/>
-      <c r="C153" s="46"/>
       <c r="D153" s="18"/>
       <c r="E153" s="18"/>
       <c r="F153" s="47"/>
     </row>
     <row r="154" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A154" s="15"/>
-      <c r="B154" s="46"/>
-      <c r="C154" s="46"/>
       <c r="D154" s="18"/>
       <c r="E154" s="18"/>
       <c r="F154" s="47"/>
     </row>
     <row r="155" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A155" s="15"/>
-      <c r="B155" s="46"/>
-      <c r="C155" s="46"/>
       <c r="D155" s="18"/>
       <c r="E155" s="18"/>
       <c r="F155" s="47"/>
     </row>
     <row r="156" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A156" s="15"/>
-      <c r="B156" s="46"/>
-      <c r="C156" s="46"/>
       <c r="D156" s="18"/>
       <c r="E156" s="18"/>
       <c r="F156" s="47"/>
@@ -15587,48 +15566,6 @@
       <c r="D321" s="18"/>
       <c r="E321" s="18"/>
       <c r="F321" s="47"/>
-    </row>
-    <row r="322" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A322" s="15"/>
-      <c r="D322" s="18"/>
-      <c r="E322" s="18"/>
-      <c r="F322" s="47"/>
-    </row>
-    <row r="323" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A323" s="15"/>
-      <c r="D323" s="18"/>
-      <c r="E323" s="18"/>
-      <c r="F323" s="47"/>
-    </row>
-    <row r="324" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A324" s="15"/>
-      <c r="D324" s="18"/>
-      <c r="E324" s="18"/>
-      <c r="F324" s="47"/>
-    </row>
-    <row r="325" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A325" s="15"/>
-      <c r="D325" s="18"/>
-      <c r="E325" s="18"/>
-      <c r="F325" s="47"/>
-    </row>
-    <row r="326" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A326" s="15"/>
-      <c r="D326" s="18"/>
-      <c r="E326" s="18"/>
-      <c r="F326" s="47"/>
-    </row>
-    <row r="327" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A327" s="15"/>
-      <c r="D327" s="18"/>
-      <c r="E327" s="18"/>
-      <c r="F327" s="47"/>
-    </row>
-    <row r="328" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A328" s="15"/>
-      <c r="D328" s="18"/>
-      <c r="E328" s="18"/>
-      <c r="F328" s="47"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15638,10 +15575,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15734,40 +15671,105 @@
       <c r="J7" s="18"/>
       <c r="K7" s="47"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="46"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="47"/>
-    </row>
-    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="40" t="s">
+    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="40" t="s">
         <v>286</v>
       </c>
-      <c r="B9" s="45"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="41" t="s">
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43" t="s">
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="J9" s="41" t="s">
+      <c r="J8" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="K9" s="44" t="s">
+      <c r="K8" s="44" t="s">
         <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>317</v>
+      </c>
+      <c r="B9" s="72"/>
+      <c r="C9" s="46" t="s">
+        <v>324</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>413</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="F9" s="47"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>328</v>
+      </c>
+      <c r="B12" s="72"/>
+      <c r="C12" s="46" t="s">
+        <v>337</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>413</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="F12" s="47"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C13" s="46" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C14" s="46" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>332</v>
+      </c>
+      <c r="B15" s="72"/>
+      <c r="C15" s="46" t="s">
+        <v>333</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>413</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="F15" s="47"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C16" s="46" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="46" t="s">
+        <v>479</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed xbee max min values. reset n_xbee on 1sec scan
sorry about that mess.
</commit_message>
<xml_diff>
--- a/CombSpillageCode.xlsx
+++ b/CombSpillageCode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sampling sequence" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2127" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2121" uniqueCount="474">
   <si>
     <t>Second</t>
   </si>
@@ -1477,24 +1477,6 @@
   </si>
   <si>
     <t>sec_count</t>
-  </si>
-  <si>
-    <t>vbatt_x005F_xbee1_min</t>
-  </si>
-  <si>
-    <t>vbatt_x005F_xbee1_max</t>
-  </si>
-  <si>
-    <t>vbatt_x005F_xbee2_min</t>
-  </si>
-  <si>
-    <t>vbatt_x005F_xbee2_max</t>
-  </si>
-  <si>
-    <t>vbatt_x005F_xbee3_min</t>
-  </si>
-  <si>
-    <t>vbatt_x005F_xbee3_max</t>
   </si>
 </sst>
 </file>
@@ -12282,10 +12264,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H321"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A114" activePane="bottomLeft" state="frozenSplit"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A105" activePane="bottomLeft" state="frozenSplit"/>
       <selection sqref="A1:A1048576"/>
-      <selection pane="bottomLeft" activeCell="C133" sqref="C133"/>
+      <selection pane="bottomLeft" activeCell="A116" sqref="A116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15575,10 +15557,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15710,67 +15692,37 @@
       </c>
       <c r="F9" s="47"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+    <row r="10" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
         <v>328</v>
       </c>
-      <c r="B12" s="72"/>
-      <c r="C12" s="46" t="s">
+      <c r="B10" s="72"/>
+      <c r="C10" s="46" t="s">
         <v>337</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D10" s="18" t="s">
         <v>413</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E10" s="18" t="s">
         <v>353</v>
       </c>
-      <c r="F12" s="47"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C13" s="46" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C14" s="46" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
+      <c r="F10" s="47"/>
+    </row>
+    <row r="11" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
         <v>332</v>
       </c>
-      <c r="B15" s="72"/>
-      <c r="C15" s="46" t="s">
+      <c r="B11" s="72"/>
+      <c r="C11" s="46" t="s">
         <v>333</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D11" s="18" t="s">
         <v>413</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="E11" s="18" t="s">
         <v>353</v>
       </c>
-      <c r="F15" s="47"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C16" s="46" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" s="46" t="s">
-        <v>479</v>
-      </c>
+      <c r="F11" s="47"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>